<commit_message>
adding a bunch of files
</commit_message>
<xml_diff>
--- a/Other_workbooks/Interneuron_density_analysis.xlsx
+++ b/Other_workbooks/Interneuron_density_analysis.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="617" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="665" uniqueCount="149">
   <si>
     <t>layered_cellFillData_p5s1crop251pt19</t>
   </si>
@@ -438,6 +438,42 @@
   </si>
   <si>
     <t>layered_cellFillData_p7s5_RL_cropped</t>
+  </si>
+  <si>
+    <t>layered_cellFillData_p5s3_PM_cropped</t>
+  </si>
+  <si>
+    <t>layered_cellFillData_p5s4_PM_cropped</t>
+  </si>
+  <si>
+    <t>layered_cellFillData_p5s5_PM_cropped</t>
+  </si>
+  <si>
+    <t>layered_cellFillData_p5s6_PM_cropped</t>
+  </si>
+  <si>
+    <t>layered_cellFillData_p6s5_PM_cropped</t>
+  </si>
+  <si>
+    <t>layered_cellFillData_p6s6_PM_cropped</t>
+  </si>
+  <si>
+    <t>layered_cellFillData_p7s1_PM_cropped</t>
+  </si>
+  <si>
+    <t>layered_cellFillData_p7s2_PM_cropped</t>
+  </si>
+  <si>
+    <t>layered_cellFillData_p7s3_PM_cropped</t>
+  </si>
+  <si>
+    <t>layered_cellFillData_p6s3_AL_cropped</t>
+  </si>
+  <si>
+    <t>layered_cellFillData_p6s4_AL_cropped</t>
+  </si>
+  <si>
+    <t>layered_cellFillData_p6s5_AL_cropped</t>
   </si>
 </sst>
 </file>
@@ -2849,10 +2885,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N73"/>
+  <dimension ref="A1:N89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="B77" sqref="B77"/>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="B81" sqref="B81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4057,59 +4093,79 @@
       <c r="J57" s="4"/>
       <c r="K57" s="4"/>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58" s="20" t="s">
         <v>80</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>121</v>
+        <v>41</v>
       </c>
       <c r="C58" s="11" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F58" s="14"/>
+      <c r="H58" s="4"/>
+      <c r="I58" s="4"/>
+      <c r="J58" s="4"/>
+      <c r="K58" s="4"/>
+    </row>
+    <row r="59" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A59" s="20" t="s">
         <v>80</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>122</v>
+        <v>42</v>
       </c>
       <c r="C59" s="11" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F59" s="14"/>
+      <c r="H59" s="4"/>
+      <c r="I59" s="4"/>
+      <c r="J59" s="4"/>
+      <c r="K59" s="4"/>
+    </row>
+    <row r="60" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60" s="20" t="s">
         <v>80</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>123</v>
+        <v>43</v>
       </c>
       <c r="C60" s="11" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F60" s="14"/>
+      <c r="H60" s="4"/>
+      <c r="I60" s="4"/>
+      <c r="J60" s="4"/>
+      <c r="K60" s="4"/>
+    </row>
+    <row r="61" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61" s="20" t="s">
         <v>80</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>124</v>
+        <v>44</v>
       </c>
       <c r="C61" s="11" t="s">
         <v>2</v>
       </c>
+      <c r="F61" s="14"/>
+      <c r="H61" s="4"/>
+      <c r="I61" s="4"/>
+      <c r="J61" s="4"/>
+      <c r="K61" s="4"/>
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62" s="20" t="s">
         <v>80</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="C62" s="11" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.25">
@@ -4117,10 +4173,10 @@
         <v>80</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="C63" s="11" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.25">
@@ -4128,108 +4184,296 @@
         <v>80</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="C64" s="11" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="20" t="s">
         <v>80</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="C65" s="11" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A66" s="20" t="s">
         <v>80</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>129</v>
+        <v>146</v>
       </c>
       <c r="C66" s="11" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="F66" s="14"/>
+    </row>
+    <row r="67" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A67" s="20" t="s">
         <v>80</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>130</v>
+        <v>147</v>
       </c>
       <c r="C67" s="11" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="F67" s="14"/>
+    </row>
+    <row r="68" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A68" s="20" t="s">
         <v>80</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>131</v>
+        <v>148</v>
       </c>
       <c r="C68" s="11" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="F68" s="14"/>
+    </row>
+    <row r="69" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A69" s="20" t="s">
         <v>80</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>132</v>
+        <v>137</v>
       </c>
       <c r="C69" s="11" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+      <c r="F69" s="14"/>
+    </row>
+    <row r="70" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A70" s="20" t="s">
         <v>80</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="C70" s="11" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+      <c r="F70" s="14"/>
+    </row>
+    <row r="71" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A71" s="20" t="s">
         <v>80</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>134</v>
+        <v>139</v>
       </c>
       <c r="C71" s="11" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+      <c r="F71" s="14"/>
+    </row>
+    <row r="72" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A72" s="20" t="s">
         <v>80</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="C72" s="11" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+      <c r="F72" s="14"/>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" s="20" t="s">
         <v>80</v>
       </c>
       <c r="B73" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="C73" s="11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A74" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C74" s="11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A75" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="C75" s="11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A76" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="C76" s="11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A77" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="C77" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="F77" s="14"/>
+    </row>
+    <row r="78" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A78" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="C78" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="F78" s="14"/>
+    </row>
+    <row r="79" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A79" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="C79" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="F79" s="14"/>
+    </row>
+    <row r="80" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A80" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="C80" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="F80" s="14"/>
+    </row>
+    <row r="81" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A81" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="C81" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="F81" s="14"/>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A82" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="C82" s="11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A83" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="C83" s="11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A84" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="C84" s="11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A85" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="C85" s="11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A86" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="C86" s="11" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A87" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C87" s="11" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A88" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C88" s="11" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A89" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="B89" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="C73" s="11" t="s">
+      <c r="C89" s="11" t="s">
         <v>46</v>
       </c>
     </row>

</xml_diff>

<commit_message>
yet another small change
</commit_message>
<xml_diff>
--- a/Other_workbooks/Interneuron_density_analysis.xlsx
+++ b/Other_workbooks/Interneuron_density_analysis.xlsx
@@ -844,8 +844,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M162"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+    <sheetView tabSelected="1" topLeftCell="A44" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G61" sqref="G61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2531,7 +2531,7 @@
         <v>1050</v>
       </c>
       <c r="G58" s="20">
-        <v>44</v>
+        <v>440</v>
       </c>
       <c r="I58" s="4"/>
       <c r="J58" s="4"/>
@@ -2560,7 +2560,7 @@
         <v>980</v>
       </c>
       <c r="G59" s="20">
-        <v>44</v>
+        <v>440</v>
       </c>
       <c r="I59" s="4"/>
       <c r="J59" s="4"/>
@@ -2589,7 +2589,7 @@
         <v>910</v>
       </c>
       <c r="G60" s="20">
-        <v>44</v>
+        <v>440</v>
       </c>
       <c r="I60" s="4"/>
       <c r="J60" s="4"/>
@@ -2618,7 +2618,7 @@
         <v>840</v>
       </c>
       <c r="G61" s="20">
-        <v>44</v>
+        <v>440</v>
       </c>
       <c r="I61" s="4"/>
       <c r="J61" s="4"/>

</xml_diff>

<commit_message>
transferred amy's notes into this master document
</commit_message>
<xml_diff>
--- a/Other_workbooks/Interneuron_density_analysis.xlsx
+++ b/Other_workbooks/Interneuron_density_analysis.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\charlie\Documents\SourceTree_local\docubase\Other_workbooks\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="22905"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11625" windowHeight="8550" activeTab="2"/>
+    <workbookView xWindow="100" yWindow="0" windowWidth="28280" windowHeight="16460" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="PVcre" sheetId="2" r:id="rId1"/>
@@ -17,8 +12,11 @@
     <sheet name="SOMcre" sheetId="5" r:id="rId3"/>
     <sheet name="Experiment Notes" sheetId="6" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
@@ -27,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="722" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="750" uniqueCount="190">
   <si>
     <t>layered_cellFillData_p5s1crop251pt19</t>
   </si>
@@ -209,9 +207,6 @@
     <t>PM Coordinates</t>
   </si>
   <si>
-    <t>AL Coordinates</t>
-  </si>
-  <si>
     <t>RL Coordinates</t>
   </si>
   <si>
@@ -230,9 +225,6 @@
     <t>SOM-Cre x Ai14</t>
   </si>
   <si>
-    <t>volume injected (nl)</t>
-  </si>
-  <si>
     <t>sex</t>
   </si>
   <si>
@@ -263,12 +255,6 @@
     <t>Alexa-488</t>
   </si>
   <si>
-    <t>50 - 120 nl</t>
-  </si>
-  <si>
-    <t>120 nl</t>
-  </si>
-  <si>
     <t>EB_150427_A</t>
   </si>
   <si>
@@ -365,9 +351,6 @@
     <t>630, 880</t>
   </si>
   <si>
-    <t>injection coordinates (um) [a/p, m/l from CC fusion]</t>
-  </si>
-  <si>
     <t>980, 1175</t>
   </si>
   <si>
@@ -531,6 +514,87 @@
   </si>
   <si>
     <t>layered_cellFillData_CH_150612_A_p5s4_ERC_cropped.mat</t>
+  </si>
+  <si>
+    <t>Surgery Notes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Burr hole 2.56 mm left of lambda, posterior edge on lamboid suture. Injected 100 nl unfloxed eGFP, 400 um deep, 50 nl/min, waited ten mins. May have injected more due to built up pressure in pipette. </t>
+  </si>
+  <si>
+    <t>AL Coordinates (um) [a/p, m/l from CC fusion]</t>
+  </si>
+  <si>
+    <t>Histology Notes</t>
+  </si>
+  <si>
+    <t>Great perfusion but possible cortical damage during extraction. 70 micron sections.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Burr hole 2.56 mm left of lambda, posterior edge on suture. Injected 100 nl unfloxed eGFP, 400 um deep, 50 nl/min, waited ten mins. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Poor perfusion quality (brain not fixed or cleared at all). 70 micron sections. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Burr hole 2.56 mm left of lambda, posterior edge on suture, some backflow during injection. 100 nl unfloxed eGFP, 400 um deep, 50 nl/min, waited ten mins. </t>
+  </si>
+  <si>
+    <t>Decent perfusion quality. 70 micron sections.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Burr hole 2.55 mm left of lambda, bottom edge right on suture. Mouse was housed alone and was a bit psycho/depressed. Mouse was 2 months old (dob 7/16/14) at time of surgery. Injected 100 nl unfloxed eGFP, 50 nl/min, 400 um deep, waited ten mins. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Decent perfusion quality, possible cortical damage during extraction (mostly on right hemisphere but possible on left as well). 70 micron sections. </t>
+  </si>
+  <si>
+    <t>Mouse was 2 months old (dob 7/16/14) at time of injection. Burr hole 2.55 mm left of lambda, bottom edge slightly anterior to suture. Injected 100 nl unfloxed eGFP, 50 nl/min, 400 um deep, waited ten mins. May have injected less than 100 nl due to appearance of an air bubble in the tip of pipette.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Decent perfusion quality. 70 micron sections. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Burr hole 2.55 mm left of lambda, slightly anterior to suture. Some bleeding in burr hole during drilling. Injected 100 nl unfloxed eGFP, 50 nl/min, 400 um deep, waited ten mins. It was hard to tell when the pipette went in the brain. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Burr hole 2.56 mm left of lambda. Some bleeding during drilling. Injected 100 nl of AAV1.chR2.TdTomato 400 microns deep, 50 nl/min, waited 10 min. Some back flow during injection. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Perfusion 4 weeks after injection instead of 3! Punctured lung but brain was still clear. Possible damage to ventral side. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Burr hole 2.55 mm left of lambda. Some bleeding during drilling. Injected 100 nl AAV9.ChR2.TdTomato 400 microns deep, 50 nl/min, waited 10 min. </t>
+  </si>
+  <si>
+    <t>Good perfusion. 70 micron sections.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Burr hole 2.55 mm left of lambda. Injected 100 nl AAV9.ChR2.TdTomato, 400 microns deep, 50 nl/min, waited 10 min. Nicked skull with scalpel. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">70 micron sections. Decent perfusion but may have damaged cortex during extraction. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Burr hole 2.55 mm left of lambda. Injected 100 nl AAV9.ChR2.TdTomato 400 microns deep, 50 nl/min, waited 10 min. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">70 micron sections. Good perfusion. </t>
+  </si>
+  <si>
+    <t>Injected 75 nl of unfloxed GFP into V1 at a flow rate of 50 nl/min. Some back flow</t>
+  </si>
+  <si>
+    <t>Injected 120 nl of Alexa-488 into V1 at a depth of 400 um. Injection site was roughly 2.57 mm left of lambda and anterior to the lamboid suture.</t>
+  </si>
+  <si>
+    <t>Injected 120 nl of Alexa-488 into V1 at a depth of 400 um.  Injection site was roughly 2.57 mm left of lambda and anterior to the lamboid suture.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Injected 50 to 120 nl of virus into V1. The exact quantity was unknown because the meniscus was difficult to see.  Injection site was roughly 2.57 mm left of lambda and anterior to the lamboid suture. Post-hoc analysis reveals massive injection site... </t>
+  </si>
+  <si>
+    <t>Injected 100 nl of virus into V1 at 350 um depth, 2.56 mm left of lambda, anterior to the lamboid suture.</t>
   </si>
 </sst>
 </file>
@@ -540,7 +604,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -552,6 +616,29 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -574,10 +661,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -619,8 +710,15 @@
     </xf>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="5">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -679,7 +777,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -714,7 +812,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -891,7 +989,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -901,27 +999,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M162"/>
   <sheetViews>
-    <sheetView topLeftCell="A44" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A44" workbookViewId="0">
       <selection activeCell="G61" sqref="G61"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="16.7109375" customWidth="1"/>
-    <col min="2" max="2" width="38.85546875" customWidth="1"/>
-    <col min="3" max="3" width="11.7109375" customWidth="1"/>
-    <col min="4" max="4" width="11.140625" customWidth="1"/>
-    <col min="6" max="6" width="21.42578125" customWidth="1"/>
+    <col min="1" max="1" width="16.6640625" customWidth="1"/>
+    <col min="2" max="2" width="38.83203125" customWidth="1"/>
+    <col min="3" max="3" width="11.6640625" customWidth="1"/>
+    <col min="4" max="4" width="11.1640625" customWidth="1"/>
+    <col min="6" max="6" width="21.5" customWidth="1"/>
     <col min="7" max="7" width="19" style="20" customWidth="1"/>
-    <col min="8" max="8" width="10.85546875" customWidth="1"/>
-    <col min="9" max="9" width="12.28515625" customWidth="1"/>
-    <col min="10" max="10" width="11.85546875" customWidth="1"/>
+    <col min="8" max="8" width="10.83203125" customWidth="1"/>
+    <col min="9" max="9" width="12.33203125" customWidth="1"/>
+    <col min="10" max="10" width="11.83203125" customWidth="1"/>
     <col min="11" max="11" width="10" customWidth="1"/>
-    <col min="12" max="12" width="10.28515625" customWidth="1"/>
-    <col min="13" max="13" width="9.7109375" customWidth="1"/>
+    <col min="12" max="12" width="10.33203125" customWidth="1"/>
+    <col min="13" max="13" width="9.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13">
       <c r="A1" s="2" t="s">
         <v>4</v>
       </c>
@@ -932,16 +1030,16 @@
         <v>5</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="E1" s="11" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="F1" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="G1" s="19" t="s">
         <v>83</v>
-      </c>
-      <c r="G1" s="19" t="s">
-        <v>87</v>
       </c>
       <c r="H1" s="2"/>
       <c r="I1" s="2"/>
@@ -950,7 +1048,7 @@
       <c r="L1" s="2"/>
       <c r="M1" s="2"/>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13">
       <c r="A2" t="s">
         <v>27</v>
       </c>
@@ -979,7 +1077,7 @@
       <c r="L2" s="4"/>
       <c r="M2" s="4"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13">
       <c r="A3" t="s">
         <v>27</v>
       </c>
@@ -1008,7 +1106,7 @@
       <c r="L3" s="4"/>
       <c r="M3" s="4"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13">
       <c r="A4" t="s">
         <v>27</v>
       </c>
@@ -1037,7 +1135,7 @@
       <c r="L4" s="4"/>
       <c r="M4" s="4"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13">
       <c r="A5" t="s">
         <v>27</v>
       </c>
@@ -1066,7 +1164,7 @@
       <c r="L5" s="4"/>
       <c r="M5" s="4"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13">
       <c r="A6" t="s">
         <v>27</v>
       </c>
@@ -1095,7 +1193,7 @@
       <c r="L6" s="4"/>
       <c r="M6" s="4"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13">
       <c r="A7" t="s">
         <v>27</v>
       </c>
@@ -1124,7 +1222,7 @@
       <c r="L7" s="4"/>
       <c r="M7" s="4"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13">
       <c r="A8" t="s">
         <v>27</v>
       </c>
@@ -1153,7 +1251,7 @@
       <c r="L8" s="4"/>
       <c r="M8" s="4"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13">
       <c r="A9" t="s">
         <v>27</v>
       </c>
@@ -1182,7 +1280,7 @@
       <c r="L9" s="4"/>
       <c r="M9" s="4"/>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13">
       <c r="A10" t="s">
         <v>27</v>
       </c>
@@ -1209,7 +1307,7 @@
       <c r="L10" s="4"/>
       <c r="M10" s="4"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13">
       <c r="A11" t="s">
         <v>27</v>
       </c>
@@ -1237,7 +1335,7 @@
       <c r="L11" s="4"/>
       <c r="M11" s="4"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13">
       <c r="A12" t="s">
         <v>27</v>
       </c>
@@ -1266,7 +1364,7 @@
       <c r="L12" s="4"/>
       <c r="M12" s="4"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13">
       <c r="A13" t="s">
         <v>27</v>
       </c>
@@ -1295,7 +1393,7 @@
       <c r="L13" s="4"/>
       <c r="M13" s="4"/>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13">
       <c r="A14" t="s">
         <v>31</v>
       </c>
@@ -1324,7 +1422,7 @@
       <c r="L14" s="4"/>
       <c r="M14" s="4"/>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13">
       <c r="A15" t="s">
         <v>31</v>
       </c>
@@ -1353,7 +1451,7 @@
       <c r="L15" s="4"/>
       <c r="M15" s="4"/>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13">
       <c r="A16" t="s">
         <v>31</v>
       </c>
@@ -1382,7 +1480,7 @@
       <c r="L16" s="4"/>
       <c r="M16" s="4"/>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13">
       <c r="A17" t="s">
         <v>31</v>
       </c>
@@ -1411,7 +1509,7 @@
       <c r="L17" s="4"/>
       <c r="M17" s="4"/>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13">
       <c r="A18" t="s">
         <v>31</v>
       </c>
@@ -1440,7 +1538,7 @@
       <c r="L18" s="4"/>
       <c r="M18" s="4"/>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13">
       <c r="A19" t="s">
         <v>31</v>
       </c>
@@ -1469,7 +1567,7 @@
       <c r="L19" s="4"/>
       <c r="M19" s="4"/>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13">
       <c r="A20" t="s">
         <v>31</v>
       </c>
@@ -1498,7 +1596,7 @@
       <c r="L20" s="4"/>
       <c r="M20" s="4"/>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13">
       <c r="A21" t="s">
         <v>31</v>
       </c>
@@ -1527,7 +1625,7 @@
       <c r="L21" s="4"/>
       <c r="M21" s="4"/>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13">
       <c r="A22" t="s">
         <v>31</v>
       </c>
@@ -1554,7 +1652,7 @@
       <c r="J22" s="4"/>
       <c r="M22" s="4"/>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13">
       <c r="A23" t="s">
         <v>31</v>
       </c>
@@ -1582,7 +1680,7 @@
       <c r="L23" s="4"/>
       <c r="M23" s="4"/>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13">
       <c r="A24" t="s">
         <v>31</v>
       </c>
@@ -1611,7 +1709,7 @@
       <c r="L24" s="4"/>
       <c r="M24" s="4"/>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13">
       <c r="A25" t="s">
         <v>31</v>
       </c>
@@ -1640,7 +1738,7 @@
       <c r="L25" s="4"/>
       <c r="M25" s="4"/>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13">
       <c r="A26" t="s">
         <v>32</v>
       </c>
@@ -1669,7 +1767,7 @@
       <c r="L26" s="4"/>
       <c r="M26" s="4"/>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13">
       <c r="A27" t="s">
         <v>32</v>
       </c>
@@ -1698,7 +1796,7 @@
       <c r="L27" s="4"/>
       <c r="M27" s="4"/>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13">
       <c r="A28" t="s">
         <v>32</v>
       </c>
@@ -1727,7 +1825,7 @@
       <c r="L28" s="4"/>
       <c r="M28" s="4"/>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13">
       <c r="A29" t="s">
         <v>32</v>
       </c>
@@ -1756,7 +1854,7 @@
       <c r="L29" s="4"/>
       <c r="M29" s="4"/>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13">
       <c r="A30" t="s">
         <v>32</v>
       </c>
@@ -1785,7 +1883,7 @@
       <c r="L30" s="4"/>
       <c r="M30" s="4"/>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13">
       <c r="A31" t="s">
         <v>32</v>
       </c>
@@ -1814,7 +1912,7 @@
       <c r="L31" s="4"/>
       <c r="M31" s="4"/>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13">
       <c r="A32" t="s">
         <v>32</v>
       </c>
@@ -1843,7 +1941,7 @@
       <c r="L32" s="4"/>
       <c r="M32" s="4"/>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13">
       <c r="A33" t="s">
         <v>32</v>
       </c>
@@ -1872,7 +1970,7 @@
       <c r="L33" s="4"/>
       <c r="M33" s="4"/>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13">
       <c r="A34" t="s">
         <v>32</v>
       </c>
@@ -1900,7 +1998,7 @@
       <c r="L34" s="4"/>
       <c r="M34" s="4"/>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13">
       <c r="A35" t="s">
         <v>32</v>
       </c>
@@ -1929,7 +2027,7 @@
       <c r="L35" s="4"/>
       <c r="M35" s="4"/>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:13">
       <c r="A36" t="s">
         <v>32</v>
       </c>
@@ -1958,7 +2056,7 @@
       <c r="L36" s="4"/>
       <c r="M36" s="4"/>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:13">
       <c r="A37" t="s">
         <v>32</v>
       </c>
@@ -1987,7 +2085,7 @@
       <c r="L37" s="4"/>
       <c r="M37" s="4"/>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:13">
       <c r="A38" t="s">
         <v>32</v>
       </c>
@@ -2016,7 +2114,7 @@
       <c r="L38" s="4"/>
       <c r="M38" s="4"/>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:13">
       <c r="A39" t="s">
         <v>32</v>
       </c>
@@ -2045,7 +2143,7 @@
       <c r="L39" s="4"/>
       <c r="M39" s="4"/>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:13">
       <c r="A40" t="s">
         <v>32</v>
       </c>
@@ -2074,7 +2172,7 @@
       <c r="L40" s="4"/>
       <c r="M40" s="4"/>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:13">
       <c r="A41" t="s">
         <v>32</v>
       </c>
@@ -2103,7 +2201,7 @@
       <c r="L41" s="4"/>
       <c r="M41" s="4"/>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:13">
       <c r="A42" t="s">
         <v>33</v>
       </c>
@@ -2132,7 +2230,7 @@
       <c r="L42" s="4"/>
       <c r="M42" s="4"/>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:13">
       <c r="A43" t="s">
         <v>33</v>
       </c>
@@ -2161,7 +2259,7 @@
       <c r="L43" s="4"/>
       <c r="M43" s="4"/>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:13">
       <c r="A44" t="s">
         <v>33</v>
       </c>
@@ -2190,7 +2288,7 @@
       <c r="L44" s="4"/>
       <c r="M44" s="4"/>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:13">
       <c r="A45" t="s">
         <v>33</v>
       </c>
@@ -2219,7 +2317,7 @@
       <c r="L45" s="4"/>
       <c r="M45" s="4"/>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:13">
       <c r="A46" t="s">
         <v>33</v>
       </c>
@@ -2248,7 +2346,7 @@
       <c r="L46" s="4"/>
       <c r="M46" s="4"/>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:13">
       <c r="A47" t="s">
         <v>33</v>
       </c>
@@ -2277,7 +2375,7 @@
       <c r="L47" s="4"/>
       <c r="M47" s="4"/>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:13">
       <c r="A48" t="s">
         <v>33</v>
       </c>
@@ -2306,7 +2404,7 @@
       <c r="L48" s="4"/>
       <c r="M48" s="4"/>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:13">
       <c r="A49" t="s">
         <v>33</v>
       </c>
@@ -2335,7 +2433,7 @@
       <c r="L49" s="4"/>
       <c r="M49" s="4"/>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:13">
       <c r="A50" t="s">
         <v>33</v>
       </c>
@@ -2364,7 +2462,7 @@
       <c r="L50" s="4"/>
       <c r="M50" s="4"/>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:13">
       <c r="A51" t="s">
         <v>33</v>
       </c>
@@ -2393,7 +2491,7 @@
       <c r="L51" s="4"/>
       <c r="M51" s="4"/>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:13">
       <c r="A52" t="s">
         <v>33</v>
       </c>
@@ -2422,7 +2520,7 @@
       <c r="L52" s="4"/>
       <c r="M52" s="4"/>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:13">
       <c r="A53" t="s">
         <v>33</v>
       </c>
@@ -2451,7 +2549,7 @@
       <c r="L53" s="4"/>
       <c r="M53" s="4"/>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:13">
       <c r="A54" t="s">
         <v>34</v>
       </c>
@@ -2480,7 +2578,7 @@
       <c r="L54" s="4"/>
       <c r="M54" s="4"/>
     </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:13">
       <c r="A55" t="s">
         <v>34</v>
       </c>
@@ -2509,7 +2607,7 @@
       <c r="L55" s="4"/>
       <c r="M55" s="4"/>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:13">
       <c r="A56" t="s">
         <v>34</v>
       </c>
@@ -2538,7 +2636,7 @@
       <c r="L56" s="4"/>
       <c r="M56" s="4"/>
     </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:13">
       <c r="A57" t="s">
         <v>34</v>
       </c>
@@ -2567,7 +2665,7 @@
       <c r="L57" s="4"/>
       <c r="M57" s="4"/>
     </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:13">
       <c r="A58" t="s">
         <v>34</v>
       </c>
@@ -2596,7 +2694,7 @@
       <c r="L58" s="4"/>
       <c r="M58" s="4"/>
     </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:13">
       <c r="A59" t="s">
         <v>34</v>
       </c>
@@ -2625,7 +2723,7 @@
       <c r="L59" s="4"/>
       <c r="M59" s="4"/>
     </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:13">
       <c r="A60" t="s">
         <v>34</v>
       </c>
@@ -2654,7 +2752,7 @@
       <c r="L60" s="4"/>
       <c r="M60" s="4"/>
     </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:13">
       <c r="A61" t="s">
         <v>34</v>
       </c>
@@ -2683,7 +2781,7 @@
       <c r="L61" s="4"/>
       <c r="M61" s="4"/>
     </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:13">
       <c r="A62" t="s">
         <v>34</v>
       </c>
@@ -2712,7 +2810,7 @@
       <c r="L62" s="4"/>
       <c r="M62" s="4"/>
     </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:13">
       <c r="A63" t="s">
         <v>34</v>
       </c>
@@ -2740,7 +2838,7 @@
       <c r="L63" s="4"/>
       <c r="M63" s="4"/>
     </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:13">
       <c r="A64" t="s">
         <v>34</v>
       </c>
@@ -2769,7 +2867,7 @@
       <c r="L64" s="4"/>
       <c r="M64" s="4"/>
     </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:13">
       <c r="A65" t="s">
         <v>34</v>
       </c>
@@ -2798,7 +2896,7 @@
       <c r="L65" s="4"/>
       <c r="M65" s="4"/>
     </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:13">
       <c r="A66" t="s">
         <v>34</v>
       </c>
@@ -2827,7 +2925,7 @@
       <c r="L66" s="4"/>
       <c r="M66" s="4"/>
     </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:13">
       <c r="A67" t="s">
         <v>34</v>
       </c>
@@ -2856,7 +2954,7 @@
       <c r="L67" s="4"/>
       <c r="M67" s="4"/>
     </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:13">
       <c r="A68" t="s">
         <v>34</v>
       </c>
@@ -2885,7 +2983,7 @@
       <c r="L68" s="4"/>
       <c r="M68" s="4"/>
     </row>
-    <row r="69" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:13">
       <c r="A69" t="s">
         <v>34</v>
       </c>
@@ -2914,7 +3012,7 @@
       <c r="L69" s="4"/>
       <c r="M69" s="4"/>
     </row>
-    <row r="70" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:13">
       <c r="A70" t="s">
         <v>35</v>
       </c>
@@ -2943,7 +3041,7 @@
       <c r="L70" s="4"/>
       <c r="M70" s="4"/>
     </row>
-    <row r="71" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:13">
       <c r="A71" t="s">
         <v>35</v>
       </c>
@@ -2972,7 +3070,7 @@
       <c r="L71" s="4"/>
       <c r="M71" s="4"/>
     </row>
-    <row r="72" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:13">
       <c r="A72" t="s">
         <v>35</v>
       </c>
@@ -3001,7 +3099,7 @@
       <c r="L72" s="4"/>
       <c r="M72" s="4"/>
     </row>
-    <row r="73" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:13">
       <c r="A73" t="s">
         <v>35</v>
       </c>
@@ -3030,7 +3128,7 @@
       <c r="L73" s="4"/>
       <c r="M73" s="4"/>
     </row>
-    <row r="74" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:13">
       <c r="A74" t="s">
         <v>35</v>
       </c>
@@ -3059,7 +3157,7 @@
       <c r="L74" s="4"/>
       <c r="M74" s="4"/>
     </row>
-    <row r="75" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:13">
       <c r="A75" t="s">
         <v>35</v>
       </c>
@@ -3088,7 +3186,7 @@
       <c r="L75" s="4"/>
       <c r="M75" s="4"/>
     </row>
-    <row r="76" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:13">
       <c r="A76" t="s">
         <v>35</v>
       </c>
@@ -3117,7 +3215,7 @@
       <c r="L76" s="4"/>
       <c r="M76" s="4"/>
     </row>
-    <row r="77" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:13">
       <c r="A77" t="s">
         <v>35</v>
       </c>
@@ -3146,7 +3244,7 @@
       <c r="L77" s="4"/>
       <c r="M77" s="4"/>
     </row>
-    <row r="78" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:13">
       <c r="A78" t="s">
         <v>35</v>
       </c>
@@ -3175,7 +3273,7 @@
       <c r="L78" s="4"/>
       <c r="M78" s="4"/>
     </row>
-    <row r="79" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:13">
       <c r="A79" t="s">
         <v>35</v>
       </c>
@@ -3204,7 +3302,7 @@
       <c r="L79" s="4"/>
       <c r="M79" s="4"/>
     </row>
-    <row r="80" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:13">
       <c r="A80" t="s">
         <v>35</v>
       </c>
@@ -3233,7 +3331,7 @@
       <c r="L80" s="4"/>
       <c r="M80" s="4"/>
     </row>
-    <row r="81" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:13">
       <c r="A81" t="s">
         <v>35</v>
       </c>
@@ -3262,225 +3360,230 @@
       <c r="L81" s="4"/>
       <c r="M81" s="4"/>
     </row>
-    <row r="87" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:13">
       <c r="M87" s="4"/>
     </row>
-    <row r="88" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:13">
       <c r="M88" s="4"/>
     </row>
-    <row r="89" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:13">
       <c r="M89" s="4"/>
     </row>
-    <row r="90" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:13">
       <c r="M90" s="4"/>
     </row>
-    <row r="91" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:13">
       <c r="M91" s="4"/>
     </row>
-    <row r="92" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:13">
       <c r="M92" s="4"/>
     </row>
-    <row r="93" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:13">
       <c r="M93" s="4"/>
     </row>
-    <row r="94" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:13">
       <c r="M94" s="4"/>
     </row>
-    <row r="99" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="99" spans="13:13">
       <c r="M99" s="4"/>
     </row>
-    <row r="100" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="100" spans="13:13">
       <c r="M100" s="4"/>
     </row>
-    <row r="101" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="101" spans="13:13">
       <c r="M101" s="4"/>
     </row>
-    <row r="102" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="102" spans="13:13">
       <c r="M102" s="4"/>
     </row>
-    <row r="103" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="103" spans="13:13">
       <c r="M103" s="4"/>
     </row>
-    <row r="104" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="104" spans="13:13">
       <c r="M104" s="4"/>
     </row>
-    <row r="105" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="105" spans="13:13">
       <c r="M105" s="4"/>
     </row>
-    <row r="106" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="106" spans="13:13">
       <c r="M106" s="4"/>
     </row>
-    <row r="107" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="107" spans="13:13">
       <c r="M107" s="4"/>
     </row>
-    <row r="108" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="108" spans="13:13">
       <c r="M108" s="4"/>
     </row>
-    <row r="109" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="109" spans="13:13">
       <c r="M109" s="4"/>
     </row>
-    <row r="110" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="110" spans="13:13">
       <c r="M110" s="4"/>
     </row>
-    <row r="111" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="111" spans="13:13">
       <c r="M111" s="4"/>
     </row>
-    <row r="112" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="112" spans="13:13">
       <c r="M112" s="4"/>
     </row>
-    <row r="113" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="113" spans="13:13">
       <c r="M113" s="4"/>
     </row>
-    <row r="114" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="114" spans="13:13">
       <c r="M114" s="4"/>
     </row>
-    <row r="115" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="115" spans="13:13">
       <c r="M115" s="4"/>
     </row>
-    <row r="116" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="116" spans="13:13">
       <c r="M116" s="4"/>
     </row>
-    <row r="117" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="117" spans="13:13">
       <c r="M117" s="4"/>
     </row>
-    <row r="118" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="118" spans="13:13">
       <c r="M118" s="4"/>
     </row>
-    <row r="119" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="119" spans="13:13">
       <c r="M119" s="4"/>
     </row>
-    <row r="120" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="120" spans="13:13">
       <c r="M120" s="4"/>
     </row>
-    <row r="121" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="121" spans="13:13">
       <c r="M121" s="4"/>
     </row>
-    <row r="122" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="122" spans="13:13">
       <c r="M122" s="4"/>
     </row>
-    <row r="123" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="123" spans="13:13">
       <c r="M123" s="4"/>
     </row>
-    <row r="124" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="124" spans="13:13">
       <c r="M124" s="4"/>
     </row>
-    <row r="125" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="125" spans="13:13">
       <c r="M125" s="4"/>
     </row>
-    <row r="126" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="126" spans="13:13">
       <c r="M126" s="4"/>
     </row>
-    <row r="127" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="127" spans="13:13">
       <c r="M127" s="4"/>
     </row>
-    <row r="128" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="128" spans="13:13">
       <c r="M128" s="4"/>
     </row>
-    <row r="129" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="129" spans="13:13">
       <c r="M129" s="4"/>
     </row>
-    <row r="130" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="130" spans="13:13">
       <c r="M130" s="4"/>
     </row>
-    <row r="131" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="131" spans="13:13">
       <c r="M131" s="4"/>
     </row>
-    <row r="132" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="132" spans="13:13">
       <c r="M132" s="4"/>
     </row>
-    <row r="133" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="133" spans="13:13">
       <c r="M133" s="4"/>
     </row>
-    <row r="134" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="134" spans="13:13">
       <c r="M134" s="4"/>
     </row>
-    <row r="135" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="135" spans="13:13">
       <c r="M135" s="4"/>
     </row>
-    <row r="136" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="136" spans="13:13">
       <c r="M136" s="4"/>
     </row>
-    <row r="137" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="137" spans="13:13">
       <c r="M137" s="4"/>
     </row>
-    <row r="138" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="138" spans="13:13">
       <c r="M138" s="4"/>
     </row>
-    <row r="139" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="139" spans="13:13">
       <c r="M139" s="4"/>
     </row>
-    <row r="140" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="140" spans="13:13">
       <c r="M140" s="4"/>
     </row>
-    <row r="141" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="141" spans="13:13">
       <c r="M141" s="4"/>
     </row>
-    <row r="142" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="142" spans="13:13">
       <c r="M142" s="4"/>
     </row>
-    <row r="143" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="143" spans="13:13">
       <c r="M143" s="4"/>
     </row>
-    <row r="144" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="144" spans="13:13">
       <c r="M144" s="4"/>
     </row>
-    <row r="145" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="145" spans="13:13">
       <c r="M145" s="4"/>
     </row>
-    <row r="146" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="146" spans="13:13">
       <c r="M146" s="4"/>
     </row>
-    <row r="147" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="147" spans="13:13">
       <c r="M147" s="4"/>
     </row>
-    <row r="148" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="148" spans="13:13">
       <c r="M148" s="4"/>
     </row>
-    <row r="149" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="149" spans="13:13">
       <c r="M149" s="4"/>
     </row>
-    <row r="150" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="150" spans="13:13">
       <c r="M150" s="4"/>
     </row>
-    <row r="151" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="151" spans="13:13">
       <c r="M151" s="4"/>
     </row>
-    <row r="152" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="152" spans="13:13">
       <c r="M152" s="4"/>
     </row>
-    <row r="153" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="153" spans="13:13">
       <c r="M153" s="4"/>
     </row>
-    <row r="154" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="154" spans="13:13">
       <c r="M154" s="4"/>
     </row>
-    <row r="155" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="155" spans="13:13">
       <c r="M155" s="4"/>
     </row>
-    <row r="156" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="156" spans="13:13">
       <c r="M156" s="4"/>
     </row>
-    <row r="157" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="157" spans="13:13">
       <c r="M157" s="4"/>
     </row>
-    <row r="158" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="158" spans="13:13">
       <c r="M158" s="4"/>
     </row>
-    <row r="159" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="159" spans="13:13">
       <c r="M159" s="4"/>
     </row>
-    <row r="160" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="160" spans="13:13">
       <c r="M160" s="4"/>
     </row>
-    <row r="161" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="161" spans="13:13">
       <c r="M161" s="4"/>
     </row>
-    <row r="162" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="162" spans="13:13">
       <c r="M162" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -3488,26 +3591,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N89"/>
   <sheetViews>
-    <sheetView topLeftCell="A73" workbookViewId="0">
+    <sheetView topLeftCell="A51" workbookViewId="0">
       <selection activeCell="F53" sqref="F53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="14.28515625" style="18" customWidth="1"/>
-    <col min="2" max="2" width="38.42578125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="13.28515625" customWidth="1"/>
-    <col min="4" max="4" width="10.5703125" style="20" customWidth="1"/>
-    <col min="6" max="6" width="19.7109375" style="20" customWidth="1"/>
-    <col min="7" max="7" width="10.7109375" customWidth="1"/>
-    <col min="8" max="8" width="12.85546875" customWidth="1"/>
-    <col min="9" max="9" width="11.5703125" customWidth="1"/>
-    <col min="10" max="10" width="10.140625" customWidth="1"/>
-    <col min="11" max="12" width="9.7109375" customWidth="1"/>
-    <col min="14" max="14" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.33203125" style="18" customWidth="1"/>
+    <col min="2" max="2" width="38.5" style="1" customWidth="1"/>
+    <col min="3" max="3" width="13.33203125" customWidth="1"/>
+    <col min="4" max="4" width="10.5" style="20" customWidth="1"/>
+    <col min="6" max="6" width="19.6640625" style="20" customWidth="1"/>
+    <col min="7" max="7" width="10.6640625" customWidth="1"/>
+    <col min="8" max="8" width="12.83203125" customWidth="1"/>
+    <col min="9" max="9" width="11.5" customWidth="1"/>
+    <col min="10" max="10" width="10.1640625" customWidth="1"/>
+    <col min="11" max="12" width="9.6640625" customWidth="1"/>
+    <col min="14" max="14" width="13.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14">
       <c r="A1" s="17" t="s">
         <v>4</v>
       </c>
@@ -3518,16 +3621,16 @@
         <v>5</v>
       </c>
       <c r="D1" s="19" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="E1" s="11" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="F1" s="19" t="s">
+        <v>79</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>83</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>87</v>
       </c>
       <c r="H1" s="2"/>
       <c r="I1" s="2"/>
@@ -3535,7 +3638,7 @@
       <c r="K1" s="2"/>
       <c r="L1" s="2"/>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14">
       <c r="A2" s="18" t="s">
         <v>1</v>
       </c>
@@ -3564,7 +3667,7 @@
       <c r="K2" s="4"/>
       <c r="N2" s="5"/>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14">
       <c r="A3" s="18" t="s">
         <v>1</v>
       </c>
@@ -3592,7 +3695,7 @@
       <c r="J3" s="4"/>
       <c r="K3" s="4"/>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14">
       <c r="A4" s="18" t="s">
         <v>1</v>
       </c>
@@ -3620,7 +3723,7 @@
       <c r="J4" s="4"/>
       <c r="K4" s="4"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14">
       <c r="A5" s="18" t="s">
         <v>1</v>
       </c>
@@ -3647,7 +3750,7 @@
       <c r="I5" s="4"/>
       <c r="J5" s="4"/>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14">
       <c r="A6" s="18" t="s">
         <v>1</v>
       </c>
@@ -3675,7 +3778,7 @@
       <c r="J6" s="4"/>
       <c r="K6" s="4"/>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14">
       <c r="A7" s="18" t="s">
         <v>1</v>
       </c>
@@ -3703,7 +3806,7 @@
       <c r="J7" s="4"/>
       <c r="K7" s="4"/>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14">
       <c r="A8" s="18" t="s">
         <v>1</v>
       </c>
@@ -3731,7 +3834,7 @@
       <c r="J8" s="4"/>
       <c r="K8" s="4"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14">
       <c r="A9" s="18" t="s">
         <v>1</v>
       </c>
@@ -3759,7 +3862,7 @@
       <c r="J9" s="4"/>
       <c r="K9" s="4"/>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14">
       <c r="A10" s="18" t="s">
         <v>1</v>
       </c>
@@ -3786,7 +3889,7 @@
       <c r="J10" s="4"/>
       <c r="L10" s="4"/>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14">
       <c r="A11" s="18" t="s">
         <v>1</v>
       </c>
@@ -3810,7 +3913,7 @@
         <v>1206</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14">
       <c r="A12" s="18" t="s">
         <v>1</v>
       </c>
@@ -3837,7 +3940,7 @@
       <c r="J12" s="4"/>
       <c r="L12" s="4"/>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14">
       <c r="A13" s="18" t="s">
         <v>1</v>
       </c>
@@ -3864,7 +3967,7 @@
       <c r="J13" s="4"/>
       <c r="K13" s="4"/>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14">
       <c r="A14" s="18" t="s">
         <v>17</v>
       </c>
@@ -3892,7 +3995,7 @@
       <c r="J14" s="4"/>
       <c r="K14" s="4"/>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14">
       <c r="A15" s="18" t="s">
         <v>17</v>
       </c>
@@ -3920,7 +4023,7 @@
       <c r="J15" s="4"/>
       <c r="K15" s="4"/>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14">
       <c r="A16" s="18" t="s">
         <v>17</v>
       </c>
@@ -3948,7 +4051,7 @@
       <c r="J16" s="4"/>
       <c r="K16" s="4"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11">
       <c r="A17" s="18" t="s">
         <v>17</v>
       </c>
@@ -3976,7 +4079,7 @@
       <c r="J17" s="4"/>
       <c r="K17" s="4"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11">
       <c r="A18" s="18" t="s">
         <v>17</v>
       </c>
@@ -4003,7 +4106,7 @@
       <c r="I18" s="4"/>
       <c r="K18" s="4"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11">
       <c r="A19" s="18" t="s">
         <v>17</v>
       </c>
@@ -4031,7 +4134,7 @@
       <c r="J19" s="4"/>
       <c r="K19" s="4"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11">
       <c r="A20" s="18" t="s">
         <v>17</v>
       </c>
@@ -4059,7 +4162,7 @@
       <c r="J20" s="4"/>
       <c r="K20" s="4"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11">
       <c r="A21" s="18" t="s">
         <v>17</v>
       </c>
@@ -4087,7 +4190,7 @@
       <c r="J21" s="4"/>
       <c r="K21" s="4"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11">
       <c r="A22" s="18" t="s">
         <v>17</v>
       </c>
@@ -4114,7 +4217,7 @@
       <c r="J22" s="4"/>
       <c r="K22" s="4"/>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11">
       <c r="A23" s="18" t="s">
         <v>17</v>
       </c>
@@ -4140,7 +4243,7 @@
       <c r="H23" s="4"/>
       <c r="K23" s="4"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11">
       <c r="A24" s="18" t="s">
         <v>17</v>
       </c>
@@ -4167,7 +4270,7 @@
       <c r="J24" s="4"/>
       <c r="K24" s="4"/>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11">
       <c r="A25" s="18" t="s">
         <v>17</v>
       </c>
@@ -4195,7 +4298,7 @@
       <c r="J25" s="4"/>
       <c r="K25" s="4"/>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11">
       <c r="A26" s="18" t="s">
         <v>17</v>
       </c>
@@ -4223,7 +4326,7 @@
       <c r="J26" s="4"/>
       <c r="K26" s="4"/>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11">
       <c r="A27" s="18" t="s">
         <v>17</v>
       </c>
@@ -4251,7 +4354,7 @@
       <c r="J27" s="4"/>
       <c r="K27" s="4"/>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11">
       <c r="A28" s="18" t="s">
         <v>17</v>
       </c>
@@ -4279,7 +4382,7 @@
       <c r="J28" s="4"/>
       <c r="K28" s="4"/>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11">
       <c r="A29" s="18" t="s">
         <v>17</v>
       </c>
@@ -4307,7 +4410,7 @@
       <c r="J29" s="4"/>
       <c r="K29" s="4"/>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11">
       <c r="A30" s="18" t="s">
         <v>18</v>
       </c>
@@ -4335,7 +4438,7 @@
       <c r="J30" s="4"/>
       <c r="K30" s="4"/>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11">
       <c r="A31" s="18" t="s">
         <v>18</v>
       </c>
@@ -4363,7 +4466,7 @@
       <c r="J31" s="4"/>
       <c r="K31" s="4"/>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11">
       <c r="A32" s="18" t="s">
         <v>18</v>
       </c>
@@ -4391,7 +4494,7 @@
       <c r="J32" s="4"/>
       <c r="K32" s="4"/>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11">
       <c r="A33" s="18" t="s">
         <v>18</v>
       </c>
@@ -4419,7 +4522,7 @@
       <c r="J33" s="4"/>
       <c r="K33" s="4"/>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11">
       <c r="A34" s="18" t="s">
         <v>18</v>
       </c>
@@ -4447,7 +4550,7 @@
       <c r="J34" s="4"/>
       <c r="K34" s="4"/>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11">
       <c r="A35" s="18" t="s">
         <v>18</v>
       </c>
@@ -4475,7 +4578,7 @@
       <c r="J35" s="4"/>
       <c r="K35" s="4"/>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11">
       <c r="A36" s="18" t="s">
         <v>18</v>
       </c>
@@ -4503,7 +4606,7 @@
       <c r="J36" s="4"/>
       <c r="K36" s="4"/>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11">
       <c r="A37" s="18" t="s">
         <v>18</v>
       </c>
@@ -4530,7 +4633,7 @@
       <c r="I37" s="4"/>
       <c r="K37" s="4"/>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11">
       <c r="A38" s="18" t="s">
         <v>18</v>
       </c>
@@ -4557,7 +4660,7 @@
       <c r="J38" s="4"/>
       <c r="K38" s="4"/>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11">
       <c r="A39" s="18" t="s">
         <v>18</v>
       </c>
@@ -4584,7 +4687,7 @@
       <c r="J39" s="4"/>
       <c r="K39" s="4"/>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11">
       <c r="A40" s="18" t="s">
         <v>18</v>
       </c>
@@ -4611,7 +4714,7 @@
       <c r="I40" s="4"/>
       <c r="J40" s="4"/>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11">
       <c r="A41" s="18" t="s">
         <v>18</v>
       </c>
@@ -4638,7 +4741,7 @@
       <c r="J41" s="4"/>
       <c r="K41" s="4"/>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11">
       <c r="A42" s="18" t="s">
         <v>18</v>
       </c>
@@ -4665,7 +4768,7 @@
       <c r="J42" s="4"/>
       <c r="K42" s="4"/>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11">
       <c r="A43" s="18" t="s">
         <v>18</v>
       </c>
@@ -4692,7 +4795,7 @@
       <c r="J43" s="4"/>
       <c r="K43" s="4"/>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11">
       <c r="A44" s="18" t="s">
         <v>18</v>
       </c>
@@ -4719,7 +4822,7 @@
       <c r="J44" s="4"/>
       <c r="K44" s="4"/>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11">
       <c r="A45" s="18" t="s">
         <v>18</v>
       </c>
@@ -4746,7 +4849,7 @@
       <c r="J45" s="4"/>
       <c r="K45" s="4"/>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11">
       <c r="A46" s="18" t="s">
         <v>19</v>
       </c>
@@ -4774,7 +4877,7 @@
       <c r="J46" s="4"/>
       <c r="K46" s="4"/>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11">
       <c r="A47" s="18" t="s">
         <v>19</v>
       </c>
@@ -4802,7 +4905,7 @@
       <c r="J47" s="4"/>
       <c r="K47" s="4"/>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11">
       <c r="A48" s="18" t="s">
         <v>19</v>
       </c>
@@ -4829,7 +4932,7 @@
       <c r="I48" s="4"/>
       <c r="J48" s="4"/>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:11">
       <c r="A49" s="18" t="s">
         <v>19</v>
       </c>
@@ -4856,7 +4959,7 @@
       <c r="I49" s="4"/>
       <c r="J49" s="4"/>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11">
       <c r="A50" s="18" t="s">
         <v>19</v>
       </c>
@@ -4884,7 +4987,7 @@
       <c r="J50" s="4"/>
       <c r="K50" s="4"/>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11">
       <c r="A51" s="18" t="s">
         <v>19</v>
       </c>
@@ -4912,7 +5015,7 @@
       <c r="J51" s="4"/>
       <c r="K51" s="4"/>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:11">
       <c r="A52" s="18" t="s">
         <v>19</v>
       </c>
@@ -4940,7 +5043,7 @@
       <c r="J52" s="4"/>
       <c r="K52" s="4"/>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:11">
       <c r="A53" s="18" t="s">
         <v>19</v>
       </c>
@@ -4968,7 +5071,7 @@
       <c r="J53" s="4"/>
       <c r="K53" s="4"/>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:11">
       <c r="A54" s="18" t="s">
         <v>19</v>
       </c>
@@ -4995,7 +5098,7 @@
       <c r="J54" s="4"/>
       <c r="K54" s="4"/>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:11">
       <c r="A55" s="18" t="s">
         <v>19</v>
       </c>
@@ -5021,7 +5124,7 @@
       <c r="H55" s="4"/>
       <c r="K55" s="4"/>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:11">
       <c r="A56" s="18" t="s">
         <v>19</v>
       </c>
@@ -5048,7 +5151,7 @@
       <c r="J56" s="4"/>
       <c r="K56" s="4"/>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:11">
       <c r="A57" s="18" t="s">
         <v>19</v>
       </c>
@@ -5076,9 +5179,9 @@
       <c r="J57" s="4"/>
       <c r="K57" s="4"/>
     </row>
-    <row r="58" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:11" s="10" customFormat="1">
       <c r="A58" s="18" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B58" s="1" t="s">
         <v>41</v>
@@ -5104,9 +5207,9 @@
       <c r="J58" s="4"/>
       <c r="K58" s="4"/>
     </row>
-    <row r="59" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:11" s="10" customFormat="1">
       <c r="A59" s="18" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B59" s="1" t="s">
         <v>42</v>
@@ -5132,9 +5235,9 @@
       <c r="J59" s="4"/>
       <c r="K59" s="4"/>
     </row>
-    <row r="60" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:11" s="10" customFormat="1">
       <c r="A60" s="18" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B60" s="1" t="s">
         <v>43</v>
@@ -5160,9 +5263,9 @@
       <c r="J60" s="4"/>
       <c r="K60" s="4"/>
     </row>
-    <row r="61" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:11" s="10" customFormat="1">
       <c r="A61" s="18" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B61" s="1" t="s">
         <v>44</v>
@@ -5188,12 +5291,12 @@
       <c r="J61" s="4"/>
       <c r="K61" s="4"/>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:11">
       <c r="A62" s="18" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="C62" s="10" t="s">
         <v>2</v>
@@ -5212,12 +5315,12 @@
         <v>904</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:11">
       <c r="A63" s="18" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="C63" s="10" t="s">
         <v>2</v>
@@ -5236,12 +5339,12 @@
         <v>940</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:11">
       <c r="A64" s="18" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="C64" s="10" t="s">
         <v>2</v>
@@ -5260,12 +5363,12 @@
         <v>920</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:7">
       <c r="A65" s="18" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="C65" s="10" t="s">
         <v>2</v>
@@ -5284,12 +5387,12 @@
         <v>910</v>
       </c>
     </row>
-    <row r="66" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:7" s="10" customFormat="1">
       <c r="A66" s="18" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="C66" s="10" t="s">
         <v>2</v>
@@ -5308,12 +5411,12 @@
         <v>908</v>
       </c>
     </row>
-    <row r="67" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:7" s="10" customFormat="1">
       <c r="A67" s="18" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="C67" s="10" t="s">
         <v>2</v>
@@ -5332,12 +5435,12 @@
         <v>891</v>
       </c>
     </row>
-    <row r="68" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:7" s="10" customFormat="1">
       <c r="A68" s="18" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="C68" s="10" t="s">
         <v>2</v>
@@ -5356,12 +5459,12 @@
         <v>895</v>
       </c>
     </row>
-    <row r="69" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:7" s="10" customFormat="1">
       <c r="A69" s="18" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="C69" s="10" t="s">
         <v>9</v>
@@ -5380,12 +5483,12 @@
         <v>376</v>
       </c>
     </row>
-    <row r="70" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:7" s="10" customFormat="1">
       <c r="A70" s="18" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="C70" s="10" t="s">
         <v>9</v>
@@ -5404,12 +5507,12 @@
         <v>370</v>
       </c>
     </row>
-    <row r="71" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:7" s="10" customFormat="1">
       <c r="A71" s="18" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="C71" s="10" t="s">
         <v>9</v>
@@ -5428,12 +5531,12 @@
         <v>360</v>
       </c>
     </row>
-    <row r="72" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:7" s="10" customFormat="1">
       <c r="A72" s="18" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="C72" s="10" t="s">
         <v>9</v>
@@ -5452,12 +5555,12 @@
         <v>373</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:7">
       <c r="A73" s="18" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="C73" s="10" t="s">
         <v>9</v>
@@ -5476,12 +5579,12 @@
         <v>372</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:7">
       <c r="A74" s="18" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="C74" s="10" t="s">
         <v>9</v>
@@ -5500,12 +5603,12 @@
         <v>381</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:7">
       <c r="A75" s="18" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="C75" s="10" t="s">
         <v>9</v>
@@ -5524,12 +5627,12 @@
         <v>380</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:7">
       <c r="A76" s="18" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="C76" s="10" t="s">
         <v>9</v>
@@ -5548,12 +5651,12 @@
         <v>375</v>
       </c>
     </row>
-    <row r="77" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:7" s="10" customFormat="1">
       <c r="A77" s="18" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="C77" s="10" t="s">
         <v>9</v>
@@ -5572,12 +5675,12 @@
         <v>381</v>
       </c>
     </row>
-    <row r="78" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:7" s="10" customFormat="1">
       <c r="A78" s="18" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="C78" s="10" t="s">
         <v>9</v>
@@ -5596,12 +5699,12 @@
         <v>375</v>
       </c>
     </row>
-    <row r="79" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:7" s="10" customFormat="1">
       <c r="A79" s="18" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="C79" s="10" t="s">
         <v>9</v>
@@ -5620,12 +5723,12 @@
         <v>385</v>
       </c>
     </row>
-    <row r="80" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:7" s="10" customFormat="1">
       <c r="A80" s="18" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="C80" s="10" t="s">
         <v>9</v>
@@ -5644,12 +5747,12 @@
         <v>388</v>
       </c>
     </row>
-    <row r="81" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:7" s="10" customFormat="1">
       <c r="A81" s="18" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="C81" s="10" t="s">
         <v>9</v>
@@ -5668,12 +5771,12 @@
         <v>390</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:7">
       <c r="A82" s="18" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="C82" s="10" t="s">
         <v>10</v>
@@ -5692,12 +5795,12 @@
         <v>1180</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:7">
       <c r="A83" s="18" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="C83" s="10" t="s">
         <v>10</v>
@@ -5716,12 +5819,12 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:7">
       <c r="A84" s="18" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="C84" s="10" t="s">
         <v>10</v>
@@ -5740,12 +5843,12 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:7">
       <c r="A85" s="18" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="C85" s="10" t="s">
         <v>10</v>
@@ -5764,12 +5867,12 @@
         <v>1210</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:7">
       <c r="A86" s="18" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="C86" s="10" t="s">
         <v>46</v>
@@ -5788,12 +5891,12 @@
         <v>850</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:7">
       <c r="A87" s="18" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="C87" s="10" t="s">
         <v>46</v>
@@ -5812,12 +5915,12 @@
         <v>870</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:7">
       <c r="A88" s="18" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="C88" s="10" t="s">
         <v>46</v>
@@ -5836,12 +5939,12 @@
         <v>840</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:7">
       <c r="A89" s="18" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="C89" s="10" t="s">
         <v>46</v>
@@ -5862,7 +5965,12 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -5870,22 +5978,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="15.140625" customWidth="1"/>
-    <col min="2" max="2" width="54.5703125" customWidth="1"/>
-    <col min="3" max="3" width="13.28515625" customWidth="1"/>
+    <col min="1" max="1" width="15.1640625" customWidth="1"/>
+    <col min="2" max="2" width="54.5" customWidth="1"/>
+    <col min="3" max="3" width="13.33203125" customWidth="1"/>
     <col min="4" max="4" width="12" customWidth="1"/>
-    <col min="5" max="5" width="10.85546875" customWidth="1"/>
-    <col min="6" max="6" width="19.5703125" customWidth="1"/>
-    <col min="7" max="7" width="15.85546875" customWidth="1"/>
+    <col min="5" max="5" width="10.83203125" customWidth="1"/>
+    <col min="6" max="6" width="19.5" customWidth="1"/>
+    <col min="7" max="7" width="15.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12">
       <c r="A1" s="2" t="s">
         <v>4</v>
       </c>
@@ -5896,16 +6004,16 @@
         <v>5</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="E1" s="11" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="F1" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="G1" s="11" t="s">
         <v>83</v>
-      </c>
-      <c r="G1" s="11" t="s">
-        <v>87</v>
       </c>
       <c r="H1" s="2"/>
       <c r="I1" s="2"/>
@@ -5913,7 +6021,7 @@
       <c r="K1" s="2"/>
       <c r="L1" s="2"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12">
       <c r="A2" t="s">
         <v>40</v>
       </c>
@@ -5937,7 +6045,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12">
       <c r="A3" t="s">
         <v>40</v>
       </c>
@@ -5961,7 +6069,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12">
       <c r="A4" t="s">
         <v>40</v>
       </c>
@@ -5985,7 +6093,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12">
       <c r="A5" t="s">
         <v>40</v>
       </c>
@@ -6009,7 +6117,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12">
       <c r="A6" t="s">
         <v>40</v>
       </c>
@@ -6033,7 +6141,7 @@
         <v>878</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12">
       <c r="A7" t="s">
         <v>40</v>
       </c>
@@ -6057,7 +6165,7 @@
         <v>878</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12">
       <c r="A8" t="s">
         <v>40</v>
       </c>
@@ -6081,7 +6189,7 @@
         <v>878</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12">
       <c r="A9" t="s">
         <v>40</v>
       </c>
@@ -6105,12 +6213,12 @@
         <v>878</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12">
       <c r="A10" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="C10" s="10" t="s">
         <v>9</v>
@@ -6129,12 +6237,12 @@
         <v>369</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12">
       <c r="A11" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="C11" s="10" t="s">
         <v>9</v>
@@ -6153,12 +6261,12 @@
         <v>364</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12">
       <c r="A12" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="C12" s="10" t="s">
         <v>9</v>
@@ -6177,12 +6285,12 @@
         <v>384</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12">
       <c r="A13" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="C13" s="10" t="s">
         <v>9</v>
@@ -6201,12 +6309,12 @@
         <v>378</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12">
       <c r="A14" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="C14" s="10" t="s">
         <v>9</v>
@@ -6225,12 +6333,12 @@
         <v>402</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12">
       <c r="A15" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="C15" s="10" t="s">
         <v>9</v>
@@ -6249,12 +6357,12 @@
         <v>386</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12">
       <c r="A16" s="10" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="C16" s="10" t="s">
         <v>9</v>
@@ -6273,12 +6381,12 @@
         <v>414</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7">
       <c r="A17" s="10" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="C17" s="10" t="s">
         <v>2</v>
@@ -6297,12 +6405,12 @@
         <v>816</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7">
       <c r="A18" s="10" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="C18" s="10" t="s">
         <v>2</v>
@@ -6321,12 +6429,12 @@
         <v>819</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7">
       <c r="A19" s="10" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="C19" s="10" t="s">
         <v>2</v>
@@ -6345,12 +6453,12 @@
         <v>811</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7">
       <c r="A20" s="10" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="C20" s="10" t="s">
         <v>2</v>
@@ -6369,90 +6477,90 @@
         <v>760</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7">
       <c r="A21" s="10" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="C21" t="s">
         <v>10</v>
       </c>
       <c r="D21" s="10"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7">
       <c r="A22" s="10" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="C22" s="10" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7">
       <c r="A23" s="10" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B23" s="10" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="C23" s="10" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7">
       <c r="A24" s="10" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B24" s="10" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="C24" s="10" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7">
       <c r="A25" s="10" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B25" s="10" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="C25" s="10" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7">
       <c r="A26" s="10" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B26" s="10" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="C26" s="10" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7">
       <c r="A27" s="10" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B27" s="10" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="C27" s="10" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7">
       <c r="A28" s="10" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B28" s="10" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C28" s="10" t="s">
         <v>10</v>
@@ -6460,7 +6568,12 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -6468,29 +6581,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" topLeftCell="G1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="I1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="62" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="15.42578125" style="6" customWidth="1"/>
+    <col min="1" max="1" width="15.5" style="6" customWidth="1"/>
     <col min="2" max="2" width="17" style="6" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" style="6" customWidth="1"/>
-    <col min="4" max="4" width="10.5703125" style="6" customWidth="1"/>
-    <col min="5" max="5" width="14.7109375" style="6" customWidth="1"/>
-    <col min="6" max="6" width="29.7109375" style="6" customWidth="1"/>
-    <col min="7" max="7" width="18.85546875" style="6" customWidth="1"/>
-    <col min="8" max="8" width="25.5703125" style="6" customWidth="1"/>
-    <col min="9" max="9" width="12.85546875" style="6" customWidth="1"/>
-    <col min="10" max="10" width="14.140625" style="6" customWidth="1"/>
-    <col min="11" max="11" width="13.140625" style="6" customWidth="1"/>
-    <col min="12" max="12" width="12.7109375" style="6" customWidth="1"/>
-    <col min="13" max="16384" width="9.140625" style="6"/>
+    <col min="3" max="3" width="9.1640625" style="6" customWidth="1"/>
+    <col min="4" max="4" width="10.5" style="6" customWidth="1"/>
+    <col min="5" max="5" width="14.6640625" style="6" customWidth="1"/>
+    <col min="6" max="6" width="29.6640625" style="6" customWidth="1"/>
+    <col min="7" max="7" width="15.5" style="6" customWidth="1"/>
+    <col min="8" max="8" width="14.1640625" style="6" customWidth="1"/>
+    <col min="9" max="9" width="13.1640625" style="6" customWidth="1"/>
+    <col min="10" max="10" width="12.6640625" style="6" customWidth="1"/>
+    <col min="11" max="11" width="52.1640625" style="6" customWidth="1"/>
+    <col min="12" max="12" width="44.6640625" style="6" customWidth="1"/>
+    <col min="13" max="16384" width="8.83203125" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="7" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" s="7" customFormat="1" ht="44" customHeight="1">
       <c r="A1" s="7" t="s">
         <v>54</v>
       </c>
@@ -6498,7 +6611,7 @@
         <v>55</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D1" s="7" t="s">
         <v>56</v>
@@ -6510,33 +6623,33 @@
         <v>58</v>
       </c>
       <c r="G1" s="7" t="s">
-        <v>67</v>
+        <v>165</v>
       </c>
       <c r="H1" s="7" t="s">
-        <v>112</v>
+        <v>59</v>
       </c>
       <c r="I1" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="J1" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="J1" s="7" t="s">
-        <v>59</v>
-      </c>
       <c r="K1" s="7" t="s">
-        <v>62</v>
+        <v>163</v>
       </c>
       <c r="L1" s="7" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" s="9" customFormat="1" ht="62" customHeight="1">
       <c r="A2" s="9" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D2" s="13">
         <v>41856</v>
@@ -6545,27 +6658,33 @@
         <v>41876</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
+      </c>
+      <c r="G2" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="H2" s="9" t="s">
+        <v>80</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>85</v>
-      </c>
-      <c r="J2" s="9" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="K2" s="9" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+        <v>177</v>
+      </c>
+      <c r="L2" s="9" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="62" customHeight="1">
       <c r="A3" s="8" t="s">
         <v>17</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D3" s="15">
         <v>41856</v>
@@ -6574,31 +6693,36 @@
         <v>41878</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="H3" s="8"/>
+        <v>70</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>85</v>
+      </c>
       <c r="I3" s="6" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="J3" s="6" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="K3" s="6" t="s">
-        <v>90</v>
+        <v>179</v>
       </c>
       <c r="L3" s="6" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="62" customHeight="1">
       <c r="A4" s="8" t="s">
         <v>18</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D4" s="15">
         <v>41856</v>
@@ -6607,31 +6731,36 @@
         <v>41878</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="H4" s="8"/>
+        <v>70</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>89</v>
+      </c>
       <c r="I4" s="6" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="J4" s="6" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="K4" s="6" t="s">
-        <v>94</v>
+        <v>181</v>
       </c>
       <c r="L4" s="6" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="62" customHeight="1">
       <c r="A5" s="8" t="s">
         <v>19</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D5" s="15">
         <v>41856</v>
@@ -6640,28 +6769,33 @@
         <v>41878</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="H5" s="8"/>
+        <v>70</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>93</v>
+      </c>
       <c r="I5" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="J5" s="6" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="K5" s="6" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+        <v>183</v>
+      </c>
+      <c r="L5" s="6" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="62" customHeight="1">
       <c r="A6" s="8" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D6" s="15">
         <v>42100</v>
@@ -6670,22 +6804,24 @@
         <v>42121</v>
       </c>
       <c r="F6" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="G6" s="6">
-        <v>100</v>
-      </c>
-      <c r="H6" s="8"/>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+      <c r="K6" s="6" t="s">
+        <v>189</v>
+      </c>
+      <c r="L6" s="6" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="62" customHeight="1">
       <c r="A7" s="8" t="s">
         <v>27</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D7" s="15">
         <v>41857</v>
@@ -6694,28 +6830,33 @@
         <v>41885</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="H7" s="8"/>
+        <v>64</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="H7" s="6" t="s">
+        <v>96</v>
+      </c>
       <c r="I7" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="J7" s="6" t="s">
-        <v>100</v>
-      </c>
-      <c r="K7" s="6" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+        <v>97</v>
+      </c>
+      <c r="K7" s="21" t="s">
+        <v>164</v>
+      </c>
+      <c r="L7" s="6" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="62" customHeight="1">
       <c r="A8" s="8" t="s">
         <v>31</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D8" s="15">
         <v>41857</v>
@@ -6724,28 +6865,33 @@
         <v>41885</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="H8" s="8"/>
+        <v>64</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>99</v>
+      </c>
       <c r="I8" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="J8" s="6" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="K8" s="6" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+        <v>168</v>
+      </c>
+      <c r="L8" s="6" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="62" customHeight="1">
       <c r="A9" s="8" t="s">
         <v>32</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D9" s="15">
         <v>41857</v>
@@ -6754,31 +6900,36 @@
         <v>41885</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="H9" s="8"/>
+        <v>64</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>102</v>
+      </c>
       <c r="I9" s="6" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="J9" s="6" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="K9" s="6" t="s">
-        <v>107</v>
+        <v>170</v>
       </c>
       <c r="L9" s="6" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="62" customHeight="1">
       <c r="A10" s="8" t="s">
         <v>33</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D10" s="15">
         <v>41836</v>
@@ -6787,28 +6938,33 @@
         <v>41900</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="H10" s="8"/>
-      <c r="I10" s="6" t="s">
-        <v>109</v>
+        <v>64</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="H10" s="6" t="s">
+        <v>106</v>
       </c>
       <c r="J10" s="6" t="s">
-        <v>110</v>
+        <v>87</v>
+      </c>
+      <c r="K10" s="6" t="s">
+        <v>172</v>
       </c>
       <c r="L10" s="6" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="92" customHeight="1">
       <c r="A11" s="8" t="s">
         <v>34</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D11" s="15">
         <v>41836</v>
@@ -6817,31 +6973,36 @@
         <v>41900</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="H11" s="8"/>
+        <v>64</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="H11" s="16" t="s">
+        <v>115</v>
+      </c>
       <c r="I11" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="J11" s="16" t="s">
-        <v>120</v>
+        <v>108</v>
+      </c>
+      <c r="J11" s="6" t="s">
+        <v>109</v>
       </c>
       <c r="K11" s="6" t="s">
-        <v>113</v>
+        <v>174</v>
       </c>
       <c r="L11" s="6" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="75" customHeight="1">
       <c r="A12" s="8" t="s">
         <v>35</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D12" s="15">
         <v>41836</v>
@@ -6850,28 +7011,33 @@
         <v>41900</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="H12" s="8"/>
+        <v>64</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="H12" s="6" t="s">
+        <v>111</v>
+      </c>
       <c r="I12" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="J12" s="6" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="K12" s="6" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+        <v>176</v>
+      </c>
+      <c r="L12" s="6" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="62" customHeight="1">
       <c r="A13" s="6" t="s">
         <v>40</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D13" s="14">
         <v>42102</v>
@@ -6880,27 +7046,30 @@
         <v>42135</v>
       </c>
       <c r="F13" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="G13" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="H13" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="K13" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="L13" s="6" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="62" customHeight="1">
+      <c r="A14" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="B14" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="G13" s="6">
-        <v>75</v>
-      </c>
-      <c r="I13" s="6" t="s">
-        <v>118</v>
-      </c>
-      <c r="J13" s="6" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>66</v>
-      </c>
       <c r="C14" s="6" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D14" s="14">
         <v>42108</v>
@@ -6909,21 +7078,24 @@
         <v>42167</v>
       </c>
       <c r="F14" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="K14" s="6" t="s">
+        <v>188</v>
+      </c>
+      <c r="L14" s="6" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="62" customHeight="1">
+      <c r="A15" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="B15" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="G14" s="6" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="B15" s="6" t="s">
-        <v>66</v>
-      </c>
       <c r="C15" s="6" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D15" s="14">
         <v>42108</v>
@@ -6932,21 +7104,24 @@
         <v>42167</v>
       </c>
       <c r="F15" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="K15" s="6" t="s">
+        <v>188</v>
+      </c>
+      <c r="L15" s="6" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="62" customHeight="1">
+      <c r="A16" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="B16" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="G15" s="6" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="B16" s="6" t="s">
-        <v>66</v>
-      </c>
       <c r="C16" s="6" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D16" s="14">
         <v>42108</v>
@@ -6955,21 +7130,24 @@
         <v>42167</v>
       </c>
       <c r="F16" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="G16" s="6" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+      <c r="K16" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="L16" s="6" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="62" customHeight="1">
       <c r="A17" s="6" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D17" s="14">
         <v>42108</v>
@@ -6978,14 +7156,22 @@
         <v>42167</v>
       </c>
       <c r="F17" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="G17" s="6" t="s">
-        <v>79</v>
+        <v>75</v>
+      </c>
+      <c r="K17" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="L17" s="6" t="s">
+        <v>184</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
some more updates to the workbook
</commit_message>
<xml_diff>
--- a/Other_workbooks/Interneuron_density_analysis.xlsx
+++ b/Other_workbooks/Interneuron_density_analysis.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="22905"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\charlie\Documents\SourceTree_local\docubase\Other_workbooks\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="100" yWindow="0" windowWidth="28280" windowHeight="16460" activeTab="3"/>
+    <workbookView xWindow="105" yWindow="0" windowWidth="28275" windowHeight="16455" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="PVcre" sheetId="2" r:id="rId1"/>
@@ -12,20 +17,20 @@
     <sheet name="SOMcre" sheetId="5" r:id="rId3"/>
     <sheet name="Experiment Notes" sheetId="6" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="152511"/>
   <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="750" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="841" uniqueCount="231">
   <si>
     <t>layered_cellFillData_p5s1crop251pt19</t>
   </si>
@@ -595,6 +600,129 @@
   </si>
   <si>
     <t>Injected 100 nl of virus into V1 at 350 um depth, 2.56 mm left of lambda, anterior to the lamboid suture.</t>
+  </si>
+  <si>
+    <t>p2s1</t>
+  </si>
+  <si>
+    <t>p2s2</t>
+  </si>
+  <si>
+    <t>p2s3</t>
+  </si>
+  <si>
+    <t>p2s4</t>
+  </si>
+  <si>
+    <t>p2s5</t>
+  </si>
+  <si>
+    <t>p2s6</t>
+  </si>
+  <si>
+    <t>p3s1</t>
+  </si>
+  <si>
+    <t>p3s2</t>
+  </si>
+  <si>
+    <t>p3s3</t>
+  </si>
+  <si>
+    <t>p3s4</t>
+  </si>
+  <si>
+    <t>p3s5</t>
+  </si>
+  <si>
+    <t>p3s6</t>
+  </si>
+  <si>
+    <t>p4s1</t>
+  </si>
+  <si>
+    <t>p4s2</t>
+  </si>
+  <si>
+    <t>p4s3</t>
+  </si>
+  <si>
+    <t>p4s4</t>
+  </si>
+  <si>
+    <t>p4s5</t>
+  </si>
+  <si>
+    <t>p4s6</t>
+  </si>
+  <si>
+    <t>p5s1</t>
+  </si>
+  <si>
+    <t>p5s2</t>
+  </si>
+  <si>
+    <t>p5s3</t>
+  </si>
+  <si>
+    <t>p5s4</t>
+  </si>
+  <si>
+    <t>p5s5</t>
+  </si>
+  <si>
+    <t>p5s6</t>
+  </si>
+  <si>
+    <t>p6s1</t>
+  </si>
+  <si>
+    <t>p6s2</t>
+  </si>
+  <si>
+    <t>p6s3</t>
+  </si>
+  <si>
+    <t>p6s4</t>
+  </si>
+  <si>
+    <t>p6s5</t>
+  </si>
+  <si>
+    <t>p6s6</t>
+  </si>
+  <si>
+    <t>lateral areas</t>
+  </si>
+  <si>
+    <t>+1</t>
+  </si>
+  <si>
+    <t>-1</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>medial areas</t>
+  </si>
+  <si>
+    <t>layered_cellFillData_CH_150612_A_p4s1_PM_cropped.mat</t>
+  </si>
+  <si>
+    <t>layered_cellFillData_CH_150612_A_p4s2_PM_cropped.mat</t>
+  </si>
+  <si>
+    <t>layered_cellFillData_CH_150612_A_p5s6_RL_cropped.mat</t>
+  </si>
+  <si>
+    <t>layered_cellFillData_CH_150612_A_p6s1_RL_cropped.mat</t>
+  </si>
+  <si>
+    <t>layered_cellFillData_CH_150612_A_p6s2_RL_cropped.mat</t>
+  </si>
+  <si>
+    <t>layered_cellFillData_CH_150612_A_p6s3_RL_cropped.mat</t>
   </si>
 </sst>
 </file>
@@ -668,7 +796,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -711,6 +839,15 @@
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -989,7 +1126,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1003,23 +1140,23 @@
       <selection activeCell="G61" sqref="G61"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.6640625" customWidth="1"/>
-    <col min="2" max="2" width="38.83203125" customWidth="1"/>
-    <col min="3" max="3" width="11.6640625" customWidth="1"/>
-    <col min="4" max="4" width="11.1640625" customWidth="1"/>
-    <col min="6" max="6" width="21.5" customWidth="1"/>
+    <col min="1" max="1" width="16.7109375" customWidth="1"/>
+    <col min="2" max="2" width="38.85546875" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" customWidth="1"/>
+    <col min="6" max="6" width="21.42578125" customWidth="1"/>
     <col min="7" max="7" width="19" style="20" customWidth="1"/>
-    <col min="8" max="8" width="10.83203125" customWidth="1"/>
-    <col min="9" max="9" width="12.33203125" customWidth="1"/>
-    <col min="10" max="10" width="11.83203125" customWidth="1"/>
+    <col min="8" max="8" width="10.85546875" customWidth="1"/>
+    <col min="9" max="9" width="12.28515625" customWidth="1"/>
+    <col min="10" max="10" width="11.85546875" customWidth="1"/>
     <col min="11" max="11" width="10" customWidth="1"/>
-    <col min="12" max="12" width="10.33203125" customWidth="1"/>
-    <col min="13" max="13" width="9.6640625" customWidth="1"/>
+    <col min="12" max="12" width="10.28515625" customWidth="1"/>
+    <col min="13" max="13" width="9.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>4</v>
       </c>
@@ -1048,7 +1185,7 @@
       <c r="L1" s="2"/>
       <c r="M1" s="2"/>
     </row>
-    <row r="2" spans="1:13">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>27</v>
       </c>
@@ -1077,7 +1214,7 @@
       <c r="L2" s="4"/>
       <c r="M2" s="4"/>
     </row>
-    <row r="3" spans="1:13">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>27</v>
       </c>
@@ -1106,7 +1243,7 @@
       <c r="L3" s="4"/>
       <c r="M3" s="4"/>
     </row>
-    <row r="4" spans="1:13">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>27</v>
       </c>
@@ -1135,7 +1272,7 @@
       <c r="L4" s="4"/>
       <c r="M4" s="4"/>
     </row>
-    <row r="5" spans="1:13">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>27</v>
       </c>
@@ -1164,7 +1301,7 @@
       <c r="L5" s="4"/>
       <c r="M5" s="4"/>
     </row>
-    <row r="6" spans="1:13">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>27</v>
       </c>
@@ -1193,7 +1330,7 @@
       <c r="L6" s="4"/>
       <c r="M6" s="4"/>
     </row>
-    <row r="7" spans="1:13">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>27</v>
       </c>
@@ -1222,7 +1359,7 @@
       <c r="L7" s="4"/>
       <c r="M7" s="4"/>
     </row>
-    <row r="8" spans="1:13">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>27</v>
       </c>
@@ -1251,7 +1388,7 @@
       <c r="L8" s="4"/>
       <c r="M8" s="4"/>
     </row>
-    <row r="9" spans="1:13">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>27</v>
       </c>
@@ -1280,7 +1417,7 @@
       <c r="L9" s="4"/>
       <c r="M9" s="4"/>
     </row>
-    <row r="10" spans="1:13">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>27</v>
       </c>
@@ -1307,7 +1444,7 @@
       <c r="L10" s="4"/>
       <c r="M10" s="4"/>
     </row>
-    <row r="11" spans="1:13">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>27</v>
       </c>
@@ -1335,7 +1472,7 @@
       <c r="L11" s="4"/>
       <c r="M11" s="4"/>
     </row>
-    <row r="12" spans="1:13">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>27</v>
       </c>
@@ -1364,7 +1501,7 @@
       <c r="L12" s="4"/>
       <c r="M12" s="4"/>
     </row>
-    <row r="13" spans="1:13">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>27</v>
       </c>
@@ -1393,7 +1530,7 @@
       <c r="L13" s="4"/>
       <c r="M13" s="4"/>
     </row>
-    <row r="14" spans="1:13">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>31</v>
       </c>
@@ -1422,7 +1559,7 @@
       <c r="L14" s="4"/>
       <c r="M14" s="4"/>
     </row>
-    <row r="15" spans="1:13">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>31</v>
       </c>
@@ -1451,7 +1588,7 @@
       <c r="L15" s="4"/>
       <c r="M15" s="4"/>
     </row>
-    <row r="16" spans="1:13">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>31</v>
       </c>
@@ -1480,7 +1617,7 @@
       <c r="L16" s="4"/>
       <c r="M16" s="4"/>
     </row>
-    <row r="17" spans="1:13">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>31</v>
       </c>
@@ -1509,7 +1646,7 @@
       <c r="L17" s="4"/>
       <c r="M17" s="4"/>
     </row>
-    <row r="18" spans="1:13">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>31</v>
       </c>
@@ -1538,7 +1675,7 @@
       <c r="L18" s="4"/>
       <c r="M18" s="4"/>
     </row>
-    <row r="19" spans="1:13">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>31</v>
       </c>
@@ -1567,7 +1704,7 @@
       <c r="L19" s="4"/>
       <c r="M19" s="4"/>
     </row>
-    <row r="20" spans="1:13">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>31</v>
       </c>
@@ -1596,7 +1733,7 @@
       <c r="L20" s="4"/>
       <c r="M20" s="4"/>
     </row>
-    <row r="21" spans="1:13">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>31</v>
       </c>
@@ -1625,7 +1762,7 @@
       <c r="L21" s="4"/>
       <c r="M21" s="4"/>
     </row>
-    <row r="22" spans="1:13">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>31</v>
       </c>
@@ -1652,7 +1789,7 @@
       <c r="J22" s="4"/>
       <c r="M22" s="4"/>
     </row>
-    <row r="23" spans="1:13">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>31</v>
       </c>
@@ -1680,7 +1817,7 @@
       <c r="L23" s="4"/>
       <c r="M23" s="4"/>
     </row>
-    <row r="24" spans="1:13">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>31</v>
       </c>
@@ -1709,7 +1846,7 @@
       <c r="L24" s="4"/>
       <c r="M24" s="4"/>
     </row>
-    <row r="25" spans="1:13">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>31</v>
       </c>
@@ -1738,7 +1875,7 @@
       <c r="L25" s="4"/>
       <c r="M25" s="4"/>
     </row>
-    <row r="26" spans="1:13">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>32</v>
       </c>
@@ -1767,7 +1904,7 @@
       <c r="L26" s="4"/>
       <c r="M26" s="4"/>
     </row>
-    <row r="27" spans="1:13">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>32</v>
       </c>
@@ -1796,7 +1933,7 @@
       <c r="L27" s="4"/>
       <c r="M27" s="4"/>
     </row>
-    <row r="28" spans="1:13">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>32</v>
       </c>
@@ -1825,7 +1962,7 @@
       <c r="L28" s="4"/>
       <c r="M28" s="4"/>
     </row>
-    <row r="29" spans="1:13">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>32</v>
       </c>
@@ -1854,7 +1991,7 @@
       <c r="L29" s="4"/>
       <c r="M29" s="4"/>
     </row>
-    <row r="30" spans="1:13">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>32</v>
       </c>
@@ -1883,7 +2020,7 @@
       <c r="L30" s="4"/>
       <c r="M30" s="4"/>
     </row>
-    <row r="31" spans="1:13">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>32</v>
       </c>
@@ -1912,7 +2049,7 @@
       <c r="L31" s="4"/>
       <c r="M31" s="4"/>
     </row>
-    <row r="32" spans="1:13">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>32</v>
       </c>
@@ -1941,7 +2078,7 @@
       <c r="L32" s="4"/>
       <c r="M32" s="4"/>
     </row>
-    <row r="33" spans="1:13">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>32</v>
       </c>
@@ -1970,7 +2107,7 @@
       <c r="L33" s="4"/>
       <c r="M33" s="4"/>
     </row>
-    <row r="34" spans="1:13">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>32</v>
       </c>
@@ -1998,7 +2135,7 @@
       <c r="L34" s="4"/>
       <c r="M34" s="4"/>
     </row>
-    <row r="35" spans="1:13">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>32</v>
       </c>
@@ -2027,7 +2164,7 @@
       <c r="L35" s="4"/>
       <c r="M35" s="4"/>
     </row>
-    <row r="36" spans="1:13">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>32</v>
       </c>
@@ -2056,7 +2193,7 @@
       <c r="L36" s="4"/>
       <c r="M36" s="4"/>
     </row>
-    <row r="37" spans="1:13">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>32</v>
       </c>
@@ -2085,7 +2222,7 @@
       <c r="L37" s="4"/>
       <c r="M37" s="4"/>
     </row>
-    <row r="38" spans="1:13">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>32</v>
       </c>
@@ -2114,7 +2251,7 @@
       <c r="L38" s="4"/>
       <c r="M38" s="4"/>
     </row>
-    <row r="39" spans="1:13">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>32</v>
       </c>
@@ -2143,7 +2280,7 @@
       <c r="L39" s="4"/>
       <c r="M39" s="4"/>
     </row>
-    <row r="40" spans="1:13">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>32</v>
       </c>
@@ -2172,7 +2309,7 @@
       <c r="L40" s="4"/>
       <c r="M40" s="4"/>
     </row>
-    <row r="41" spans="1:13">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>32</v>
       </c>
@@ -2201,7 +2338,7 @@
       <c r="L41" s="4"/>
       <c r="M41" s="4"/>
     </row>
-    <row r="42" spans="1:13">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>33</v>
       </c>
@@ -2230,7 +2367,7 @@
       <c r="L42" s="4"/>
       <c r="M42" s="4"/>
     </row>
-    <row r="43" spans="1:13">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>33</v>
       </c>
@@ -2259,7 +2396,7 @@
       <c r="L43" s="4"/>
       <c r="M43" s="4"/>
     </row>
-    <row r="44" spans="1:13">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>33</v>
       </c>
@@ -2288,7 +2425,7 @@
       <c r="L44" s="4"/>
       <c r="M44" s="4"/>
     </row>
-    <row r="45" spans="1:13">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>33</v>
       </c>
@@ -2317,7 +2454,7 @@
       <c r="L45" s="4"/>
       <c r="M45" s="4"/>
     </row>
-    <row r="46" spans="1:13">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>33</v>
       </c>
@@ -2346,7 +2483,7 @@
       <c r="L46" s="4"/>
       <c r="M46" s="4"/>
     </row>
-    <row r="47" spans="1:13">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>33</v>
       </c>
@@ -2375,7 +2512,7 @@
       <c r="L47" s="4"/>
       <c r="M47" s="4"/>
     </row>
-    <row r="48" spans="1:13">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>33</v>
       </c>
@@ -2404,7 +2541,7 @@
       <c r="L48" s="4"/>
       <c r="M48" s="4"/>
     </row>
-    <row r="49" spans="1:13">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>33</v>
       </c>
@@ -2433,7 +2570,7 @@
       <c r="L49" s="4"/>
       <c r="M49" s="4"/>
     </row>
-    <row r="50" spans="1:13">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>33</v>
       </c>
@@ -2462,7 +2599,7 @@
       <c r="L50" s="4"/>
       <c r="M50" s="4"/>
     </row>
-    <row r="51" spans="1:13">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>33</v>
       </c>
@@ -2491,7 +2628,7 @@
       <c r="L51" s="4"/>
       <c r="M51" s="4"/>
     </row>
-    <row r="52" spans="1:13">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>33</v>
       </c>
@@ -2520,7 +2657,7 @@
       <c r="L52" s="4"/>
       <c r="M52" s="4"/>
     </row>
-    <row r="53" spans="1:13">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>33</v>
       </c>
@@ -2549,7 +2686,7 @@
       <c r="L53" s="4"/>
       <c r="M53" s="4"/>
     </row>
-    <row r="54" spans="1:13">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>34</v>
       </c>
@@ -2578,7 +2715,7 @@
       <c r="L54" s="4"/>
       <c r="M54" s="4"/>
     </row>
-    <row r="55" spans="1:13">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>34</v>
       </c>
@@ -2607,7 +2744,7 @@
       <c r="L55" s="4"/>
       <c r="M55" s="4"/>
     </row>
-    <row r="56" spans="1:13">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>34</v>
       </c>
@@ -2636,7 +2773,7 @@
       <c r="L56" s="4"/>
       <c r="M56" s="4"/>
     </row>
-    <row r="57" spans="1:13">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>34</v>
       </c>
@@ -2665,7 +2802,7 @@
       <c r="L57" s="4"/>
       <c r="M57" s="4"/>
     </row>
-    <row r="58" spans="1:13">
+    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>34</v>
       </c>
@@ -2694,7 +2831,7 @@
       <c r="L58" s="4"/>
       <c r="M58" s="4"/>
     </row>
-    <row r="59" spans="1:13">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>34</v>
       </c>
@@ -2723,7 +2860,7 @@
       <c r="L59" s="4"/>
       <c r="M59" s="4"/>
     </row>
-    <row r="60" spans="1:13">
+    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>34</v>
       </c>
@@ -2752,7 +2889,7 @@
       <c r="L60" s="4"/>
       <c r="M60" s="4"/>
     </row>
-    <row r="61" spans="1:13">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>34</v>
       </c>
@@ -2781,7 +2918,7 @@
       <c r="L61" s="4"/>
       <c r="M61" s="4"/>
     </row>
-    <row r="62" spans="1:13">
+    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>34</v>
       </c>
@@ -2810,7 +2947,7 @@
       <c r="L62" s="4"/>
       <c r="M62" s="4"/>
     </row>
-    <row r="63" spans="1:13">
+    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>34</v>
       </c>
@@ -2838,7 +2975,7 @@
       <c r="L63" s="4"/>
       <c r="M63" s="4"/>
     </row>
-    <row r="64" spans="1:13">
+    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>34</v>
       </c>
@@ -2867,7 +3004,7 @@
       <c r="L64" s="4"/>
       <c r="M64" s="4"/>
     </row>
-    <row r="65" spans="1:13">
+    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>34</v>
       </c>
@@ -2896,7 +3033,7 @@
       <c r="L65" s="4"/>
       <c r="M65" s="4"/>
     </row>
-    <row r="66" spans="1:13">
+    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>34</v>
       </c>
@@ -2925,7 +3062,7 @@
       <c r="L66" s="4"/>
       <c r="M66" s="4"/>
     </row>
-    <row r="67" spans="1:13">
+    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>34</v>
       </c>
@@ -2954,7 +3091,7 @@
       <c r="L67" s="4"/>
       <c r="M67" s="4"/>
     </row>
-    <row r="68" spans="1:13">
+    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>34</v>
       </c>
@@ -2983,7 +3120,7 @@
       <c r="L68" s="4"/>
       <c r="M68" s="4"/>
     </row>
-    <row r="69" spans="1:13">
+    <row r="69" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>34</v>
       </c>
@@ -3012,7 +3149,7 @@
       <c r="L69" s="4"/>
       <c r="M69" s="4"/>
     </row>
-    <row r="70" spans="1:13">
+    <row r="70" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>35</v>
       </c>
@@ -3041,7 +3178,7 @@
       <c r="L70" s="4"/>
       <c r="M70" s="4"/>
     </row>
-    <row r="71" spans="1:13">
+    <row r="71" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>35</v>
       </c>
@@ -3070,7 +3207,7 @@
       <c r="L71" s="4"/>
       <c r="M71" s="4"/>
     </row>
-    <row r="72" spans="1:13">
+    <row r="72" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>35</v>
       </c>
@@ -3099,7 +3236,7 @@
       <c r="L72" s="4"/>
       <c r="M72" s="4"/>
     </row>
-    <row r="73" spans="1:13">
+    <row r="73" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>35</v>
       </c>
@@ -3128,7 +3265,7 @@
       <c r="L73" s="4"/>
       <c r="M73" s="4"/>
     </row>
-    <row r="74" spans="1:13">
+    <row r="74" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>35</v>
       </c>
@@ -3157,7 +3294,7 @@
       <c r="L74" s="4"/>
       <c r="M74" s="4"/>
     </row>
-    <row r="75" spans="1:13">
+    <row r="75" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>35</v>
       </c>
@@ -3186,7 +3323,7 @@
       <c r="L75" s="4"/>
       <c r="M75" s="4"/>
     </row>
-    <row r="76" spans="1:13">
+    <row r="76" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>35</v>
       </c>
@@ -3215,7 +3352,7 @@
       <c r="L76" s="4"/>
       <c r="M76" s="4"/>
     </row>
-    <row r="77" spans="1:13">
+    <row r="77" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>35</v>
       </c>
@@ -3244,7 +3381,7 @@
       <c r="L77" s="4"/>
       <c r="M77" s="4"/>
     </row>
-    <row r="78" spans="1:13">
+    <row r="78" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>35</v>
       </c>
@@ -3273,7 +3410,7 @@
       <c r="L78" s="4"/>
       <c r="M78" s="4"/>
     </row>
-    <row r="79" spans="1:13">
+    <row r="79" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>35</v>
       </c>
@@ -3302,7 +3439,7 @@
       <c r="L79" s="4"/>
       <c r="M79" s="4"/>
     </row>
-    <row r="80" spans="1:13">
+    <row r="80" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>35</v>
       </c>
@@ -3331,7 +3468,7 @@
       <c r="L80" s="4"/>
       <c r="M80" s="4"/>
     </row>
-    <row r="81" spans="1:13">
+    <row r="81" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>35</v>
       </c>
@@ -3360,220 +3497,220 @@
       <c r="L81" s="4"/>
       <c r="M81" s="4"/>
     </row>
-    <row r="87" spans="1:13">
+    <row r="87" spans="1:13" x14ac:dyDescent="0.25">
       <c r="M87" s="4"/>
     </row>
-    <row r="88" spans="1:13">
+    <row r="88" spans="1:13" x14ac:dyDescent="0.25">
       <c r="M88" s="4"/>
     </row>
-    <row r="89" spans="1:13">
+    <row r="89" spans="1:13" x14ac:dyDescent="0.25">
       <c r="M89" s="4"/>
     </row>
-    <row r="90" spans="1:13">
+    <row r="90" spans="1:13" x14ac:dyDescent="0.25">
       <c r="M90" s="4"/>
     </row>
-    <row r="91" spans="1:13">
+    <row r="91" spans="1:13" x14ac:dyDescent="0.25">
       <c r="M91" s="4"/>
     </row>
-    <row r="92" spans="1:13">
+    <row r="92" spans="1:13" x14ac:dyDescent="0.25">
       <c r="M92" s="4"/>
     </row>
-    <row r="93" spans="1:13">
+    <row r="93" spans="1:13" x14ac:dyDescent="0.25">
       <c r="M93" s="4"/>
     </row>
-    <row r="94" spans="1:13">
+    <row r="94" spans="1:13" x14ac:dyDescent="0.25">
       <c r="M94" s="4"/>
     </row>
-    <row r="99" spans="13:13">
+    <row r="99" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M99" s="4"/>
     </row>
-    <row r="100" spans="13:13">
+    <row r="100" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M100" s="4"/>
     </row>
-    <row r="101" spans="13:13">
+    <row r="101" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M101" s="4"/>
     </row>
-    <row r="102" spans="13:13">
+    <row r="102" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M102" s="4"/>
     </row>
-    <row r="103" spans="13:13">
+    <row r="103" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M103" s="4"/>
     </row>
-    <row r="104" spans="13:13">
+    <row r="104" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M104" s="4"/>
     </row>
-    <row r="105" spans="13:13">
+    <row r="105" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M105" s="4"/>
     </row>
-    <row r="106" spans="13:13">
+    <row r="106" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M106" s="4"/>
     </row>
-    <row r="107" spans="13:13">
+    <row r="107" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M107" s="4"/>
     </row>
-    <row r="108" spans="13:13">
+    <row r="108" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M108" s="4"/>
     </row>
-    <row r="109" spans="13:13">
+    <row r="109" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M109" s="4"/>
     </row>
-    <row r="110" spans="13:13">
+    <row r="110" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M110" s="4"/>
     </row>
-    <row r="111" spans="13:13">
+    <row r="111" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M111" s="4"/>
     </row>
-    <row r="112" spans="13:13">
+    <row r="112" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M112" s="4"/>
     </row>
-    <row r="113" spans="13:13">
+    <row r="113" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M113" s="4"/>
     </row>
-    <row r="114" spans="13:13">
+    <row r="114" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M114" s="4"/>
     </row>
-    <row r="115" spans="13:13">
+    <row r="115" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M115" s="4"/>
     </row>
-    <row r="116" spans="13:13">
+    <row r="116" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M116" s="4"/>
     </row>
-    <row r="117" spans="13:13">
+    <row r="117" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M117" s="4"/>
     </row>
-    <row r="118" spans="13:13">
+    <row r="118" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M118" s="4"/>
     </row>
-    <row r="119" spans="13:13">
+    <row r="119" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M119" s="4"/>
     </row>
-    <row r="120" spans="13:13">
+    <row r="120" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M120" s="4"/>
     </row>
-    <row r="121" spans="13:13">
+    <row r="121" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M121" s="4"/>
     </row>
-    <row r="122" spans="13:13">
+    <row r="122" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M122" s="4"/>
     </row>
-    <row r="123" spans="13:13">
+    <row r="123" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M123" s="4"/>
     </row>
-    <row r="124" spans="13:13">
+    <row r="124" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M124" s="4"/>
     </row>
-    <row r="125" spans="13:13">
+    <row r="125" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M125" s="4"/>
     </row>
-    <row r="126" spans="13:13">
+    <row r="126" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M126" s="4"/>
     </row>
-    <row r="127" spans="13:13">
+    <row r="127" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M127" s="4"/>
     </row>
-    <row r="128" spans="13:13">
+    <row r="128" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M128" s="4"/>
     </row>
-    <row r="129" spans="13:13">
+    <row r="129" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M129" s="4"/>
     </row>
-    <row r="130" spans="13:13">
+    <row r="130" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M130" s="4"/>
     </row>
-    <row r="131" spans="13:13">
+    <row r="131" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M131" s="4"/>
     </row>
-    <row r="132" spans="13:13">
+    <row r="132" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M132" s="4"/>
     </row>
-    <row r="133" spans="13:13">
+    <row r="133" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M133" s="4"/>
     </row>
-    <row r="134" spans="13:13">
+    <row r="134" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M134" s="4"/>
     </row>
-    <row r="135" spans="13:13">
+    <row r="135" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M135" s="4"/>
     </row>
-    <row r="136" spans="13:13">
+    <row r="136" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M136" s="4"/>
     </row>
-    <row r="137" spans="13:13">
+    <row r="137" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M137" s="4"/>
     </row>
-    <row r="138" spans="13:13">
+    <row r="138" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M138" s="4"/>
     </row>
-    <row r="139" spans="13:13">
+    <row r="139" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M139" s="4"/>
     </row>
-    <row r="140" spans="13:13">
+    <row r="140" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M140" s="4"/>
     </row>
-    <row r="141" spans="13:13">
+    <row r="141" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M141" s="4"/>
     </row>
-    <row r="142" spans="13:13">
+    <row r="142" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M142" s="4"/>
     </row>
-    <row r="143" spans="13:13">
+    <row r="143" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M143" s="4"/>
     </row>
-    <row r="144" spans="13:13">
+    <row r="144" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M144" s="4"/>
     </row>
-    <row r="145" spans="13:13">
+    <row r="145" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M145" s="4"/>
     </row>
-    <row r="146" spans="13:13">
+    <row r="146" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M146" s="4"/>
     </row>
-    <row r="147" spans="13:13">
+    <row r="147" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M147" s="4"/>
     </row>
-    <row r="148" spans="13:13">
+    <row r="148" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M148" s="4"/>
     </row>
-    <row r="149" spans="13:13">
+    <row r="149" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M149" s="4"/>
     </row>
-    <row r="150" spans="13:13">
+    <row r="150" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M150" s="4"/>
     </row>
-    <row r="151" spans="13:13">
+    <row r="151" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M151" s="4"/>
     </row>
-    <row r="152" spans="13:13">
+    <row r="152" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M152" s="4"/>
     </row>
-    <row r="153" spans="13:13">
+    <row r="153" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M153" s="4"/>
     </row>
-    <row r="154" spans="13:13">
+    <row r="154" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M154" s="4"/>
     </row>
-    <row r="155" spans="13:13">
+    <row r="155" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M155" s="4"/>
     </row>
-    <row r="156" spans="13:13">
+    <row r="156" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M156" s="4"/>
     </row>
-    <row r="157" spans="13:13">
+    <row r="157" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M157" s="4"/>
     </row>
-    <row r="158" spans="13:13">
+    <row r="158" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M158" s="4"/>
     </row>
-    <row r="159" spans="13:13">
+    <row r="159" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M159" s="4"/>
     </row>
-    <row r="160" spans="13:13">
+    <row r="160" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M160" s="4"/>
     </row>
-    <row r="161" spans="13:13">
+    <row r="161" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M161" s="4"/>
     </row>
-    <row r="162" spans="13:13">
+    <row r="162" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M162" s="4"/>
     </row>
   </sheetData>
@@ -3591,26 +3728,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N89"/>
   <sheetViews>
-    <sheetView topLeftCell="A51" workbookViewId="0">
-      <selection activeCell="F53" sqref="F53"/>
+    <sheetView topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="D81" sqref="D81"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.33203125" style="18" customWidth="1"/>
-    <col min="2" max="2" width="38.5" style="1" customWidth="1"/>
-    <col min="3" max="3" width="13.33203125" customWidth="1"/>
-    <col min="4" max="4" width="10.5" style="20" customWidth="1"/>
-    <col min="6" max="6" width="19.6640625" style="20" customWidth="1"/>
-    <col min="7" max="7" width="10.6640625" customWidth="1"/>
-    <col min="8" max="8" width="12.83203125" customWidth="1"/>
-    <col min="9" max="9" width="11.5" customWidth="1"/>
-    <col min="10" max="10" width="10.1640625" customWidth="1"/>
-    <col min="11" max="12" width="9.6640625" customWidth="1"/>
-    <col min="14" max="14" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.28515625" style="18" customWidth="1"/>
+    <col min="2" max="2" width="38.42578125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" customWidth="1"/>
+    <col min="4" max="4" width="10.42578125" style="20" customWidth="1"/>
+    <col min="6" max="6" width="19.7109375" style="20" customWidth="1"/>
+    <col min="7" max="7" width="10.7109375" customWidth="1"/>
+    <col min="8" max="8" width="12.85546875" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" customWidth="1"/>
+    <col min="10" max="10" width="10.140625" customWidth="1"/>
+    <col min="11" max="12" width="9.7109375" customWidth="1"/>
+    <col min="14" max="14" width="13.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="17" t="s">
         <v>4</v>
       </c>
@@ -3638,7 +3775,7 @@
       <c r="K1" s="2"/>
       <c r="L1" s="2"/>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>1</v>
       </c>
@@ -3667,7 +3804,7 @@
       <c r="K2" s="4"/>
       <c r="N2" s="5"/>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
         <v>1</v>
       </c>
@@ -3695,7 +3832,7 @@
       <c r="J3" s="4"/>
       <c r="K3" s="4"/>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
         <v>1</v>
       </c>
@@ -3723,7 +3860,7 @@
       <c r="J4" s="4"/>
       <c r="K4" s="4"/>
     </row>
-    <row r="5" spans="1:14">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="18" t="s">
         <v>1</v>
       </c>
@@ -3750,7 +3887,7 @@
       <c r="I5" s="4"/>
       <c r="J5" s="4"/>
     </row>
-    <row r="6" spans="1:14">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="18" t="s">
         <v>1</v>
       </c>
@@ -3778,7 +3915,7 @@
       <c r="J6" s="4"/>
       <c r="K6" s="4"/>
     </row>
-    <row r="7" spans="1:14">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="18" t="s">
         <v>1</v>
       </c>
@@ -3806,7 +3943,7 @@
       <c r="J7" s="4"/>
       <c r="K7" s="4"/>
     </row>
-    <row r="8" spans="1:14">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="18" t="s">
         <v>1</v>
       </c>
@@ -3834,7 +3971,7 @@
       <c r="J8" s="4"/>
       <c r="K8" s="4"/>
     </row>
-    <row r="9" spans="1:14">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="18" t="s">
         <v>1</v>
       </c>
@@ -3862,7 +3999,7 @@
       <c r="J9" s="4"/>
       <c r="K9" s="4"/>
     </row>
-    <row r="10" spans="1:14">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="18" t="s">
         <v>1</v>
       </c>
@@ -3889,7 +4026,7 @@
       <c r="J10" s="4"/>
       <c r="L10" s="4"/>
     </row>
-    <row r="11" spans="1:14">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="18" t="s">
         <v>1</v>
       </c>
@@ -3913,7 +4050,7 @@
         <v>1206</v>
       </c>
     </row>
-    <row r="12" spans="1:14">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="18" t="s">
         <v>1</v>
       </c>
@@ -3940,7 +4077,7 @@
       <c r="J12" s="4"/>
       <c r="L12" s="4"/>
     </row>
-    <row r="13" spans="1:14">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="18" t="s">
         <v>1</v>
       </c>
@@ -3967,7 +4104,7 @@
       <c r="J13" s="4"/>
       <c r="K13" s="4"/>
     </row>
-    <row r="14" spans="1:14">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="18" t="s">
         <v>17</v>
       </c>
@@ -3995,7 +4132,7 @@
       <c r="J14" s="4"/>
       <c r="K14" s="4"/>
     </row>
-    <row r="15" spans="1:14">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="18" t="s">
         <v>17</v>
       </c>
@@ -4023,7 +4160,7 @@
       <c r="J15" s="4"/>
       <c r="K15" s="4"/>
     </row>
-    <row r="16" spans="1:14">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="18" t="s">
         <v>17</v>
       </c>
@@ -4051,7 +4188,7 @@
       <c r="J16" s="4"/>
       <c r="K16" s="4"/>
     </row>
-    <row r="17" spans="1:11">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="18" t="s">
         <v>17</v>
       </c>
@@ -4079,7 +4216,7 @@
       <c r="J17" s="4"/>
       <c r="K17" s="4"/>
     </row>
-    <row r="18" spans="1:11">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="18" t="s">
         <v>17</v>
       </c>
@@ -4106,7 +4243,7 @@
       <c r="I18" s="4"/>
       <c r="K18" s="4"/>
     </row>
-    <row r="19" spans="1:11">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="18" t="s">
         <v>17</v>
       </c>
@@ -4134,7 +4271,7 @@
       <c r="J19" s="4"/>
       <c r="K19" s="4"/>
     </row>
-    <row r="20" spans="1:11">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="18" t="s">
         <v>17</v>
       </c>
@@ -4162,7 +4299,7 @@
       <c r="J20" s="4"/>
       <c r="K20" s="4"/>
     </row>
-    <row r="21" spans="1:11">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="18" t="s">
         <v>17</v>
       </c>
@@ -4190,7 +4327,7 @@
       <c r="J21" s="4"/>
       <c r="K21" s="4"/>
     </row>
-    <row r="22" spans="1:11">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="18" t="s">
         <v>17</v>
       </c>
@@ -4217,7 +4354,7 @@
       <c r="J22" s="4"/>
       <c r="K22" s="4"/>
     </row>
-    <row r="23" spans="1:11">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="18" t="s">
         <v>17</v>
       </c>
@@ -4243,7 +4380,7 @@
       <c r="H23" s="4"/>
       <c r="K23" s="4"/>
     </row>
-    <row r="24" spans="1:11">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="18" t="s">
         <v>17</v>
       </c>
@@ -4270,7 +4407,7 @@
       <c r="J24" s="4"/>
       <c r="K24" s="4"/>
     </row>
-    <row r="25" spans="1:11">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="18" t="s">
         <v>17</v>
       </c>
@@ -4298,7 +4435,7 @@
       <c r="J25" s="4"/>
       <c r="K25" s="4"/>
     </row>
-    <row r="26" spans="1:11">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="18" t="s">
         <v>17</v>
       </c>
@@ -4326,7 +4463,7 @@
       <c r="J26" s="4"/>
       <c r="K26" s="4"/>
     </row>
-    <row r="27" spans="1:11">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="18" t="s">
         <v>17</v>
       </c>
@@ -4354,7 +4491,7 @@
       <c r="J27" s="4"/>
       <c r="K27" s="4"/>
     </row>
-    <row r="28" spans="1:11">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="18" t="s">
         <v>17</v>
       </c>
@@ -4382,7 +4519,7 @@
       <c r="J28" s="4"/>
       <c r="K28" s="4"/>
     </row>
-    <row r="29" spans="1:11">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="18" t="s">
         <v>17</v>
       </c>
@@ -4410,7 +4547,7 @@
       <c r="J29" s="4"/>
       <c r="K29" s="4"/>
     </row>
-    <row r="30" spans="1:11">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="18" t="s">
         <v>18</v>
       </c>
@@ -4438,7 +4575,7 @@
       <c r="J30" s="4"/>
       <c r="K30" s="4"/>
     </row>
-    <row r="31" spans="1:11">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="18" t="s">
         <v>18</v>
       </c>
@@ -4466,7 +4603,7 @@
       <c r="J31" s="4"/>
       <c r="K31" s="4"/>
     </row>
-    <row r="32" spans="1:11">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="18" t="s">
         <v>18</v>
       </c>
@@ -4494,7 +4631,7 @@
       <c r="J32" s="4"/>
       <c r="K32" s="4"/>
     </row>
-    <row r="33" spans="1:11">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="18" t="s">
         <v>18</v>
       </c>
@@ -4522,7 +4659,7 @@
       <c r="J33" s="4"/>
       <c r="K33" s="4"/>
     </row>
-    <row r="34" spans="1:11">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="18" t="s">
         <v>18</v>
       </c>
@@ -4550,7 +4687,7 @@
       <c r="J34" s="4"/>
       <c r="K34" s="4"/>
     </row>
-    <row r="35" spans="1:11">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="18" t="s">
         <v>18</v>
       </c>
@@ -4578,7 +4715,7 @@
       <c r="J35" s="4"/>
       <c r="K35" s="4"/>
     </row>
-    <row r="36" spans="1:11">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="18" t="s">
         <v>18</v>
       </c>
@@ -4606,7 +4743,7 @@
       <c r="J36" s="4"/>
       <c r="K36" s="4"/>
     </row>
-    <row r="37" spans="1:11">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="18" t="s">
         <v>18</v>
       </c>
@@ -4633,7 +4770,7 @@
       <c r="I37" s="4"/>
       <c r="K37" s="4"/>
     </row>
-    <row r="38" spans="1:11">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="18" t="s">
         <v>18</v>
       </c>
@@ -4660,7 +4797,7 @@
       <c r="J38" s="4"/>
       <c r="K38" s="4"/>
     </row>
-    <row r="39" spans="1:11">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="18" t="s">
         <v>18</v>
       </c>
@@ -4687,7 +4824,7 @@
       <c r="J39" s="4"/>
       <c r="K39" s="4"/>
     </row>
-    <row r="40" spans="1:11">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="18" t="s">
         <v>18</v>
       </c>
@@ -4714,7 +4851,7 @@
       <c r="I40" s="4"/>
       <c r="J40" s="4"/>
     </row>
-    <row r="41" spans="1:11">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="18" t="s">
         <v>18</v>
       </c>
@@ -4741,7 +4878,7 @@
       <c r="J41" s="4"/>
       <c r="K41" s="4"/>
     </row>
-    <row r="42" spans="1:11">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" s="18" t="s">
         <v>18</v>
       </c>
@@ -4768,7 +4905,7 @@
       <c r="J42" s="4"/>
       <c r="K42" s="4"/>
     </row>
-    <row r="43" spans="1:11">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" s="18" t="s">
         <v>18</v>
       </c>
@@ -4795,7 +4932,7 @@
       <c r="J43" s="4"/>
       <c r="K43" s="4"/>
     </row>
-    <row r="44" spans="1:11">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="18" t="s">
         <v>18</v>
       </c>
@@ -4822,7 +4959,7 @@
       <c r="J44" s="4"/>
       <c r="K44" s="4"/>
     </row>
-    <row r="45" spans="1:11">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" s="18" t="s">
         <v>18</v>
       </c>
@@ -4849,7 +4986,7 @@
       <c r="J45" s="4"/>
       <c r="K45" s="4"/>
     </row>
-    <row r="46" spans="1:11">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" s="18" t="s">
         <v>19</v>
       </c>
@@ -4877,7 +5014,7 @@
       <c r="J46" s="4"/>
       <c r="K46" s="4"/>
     </row>
-    <row r="47" spans="1:11">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" s="18" t="s">
         <v>19</v>
       </c>
@@ -4905,7 +5042,7 @@
       <c r="J47" s="4"/>
       <c r="K47" s="4"/>
     </row>
-    <row r="48" spans="1:11">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" s="18" t="s">
         <v>19</v>
       </c>
@@ -4932,7 +5069,7 @@
       <c r="I48" s="4"/>
       <c r="J48" s="4"/>
     </row>
-    <row r="49" spans="1:11">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" s="18" t="s">
         <v>19</v>
       </c>
@@ -4959,7 +5096,7 @@
       <c r="I49" s="4"/>
       <c r="J49" s="4"/>
     </row>
-    <row r="50" spans="1:11">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" s="18" t="s">
         <v>19</v>
       </c>
@@ -4987,7 +5124,7 @@
       <c r="J50" s="4"/>
       <c r="K50" s="4"/>
     </row>
-    <row r="51" spans="1:11">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" s="18" t="s">
         <v>19</v>
       </c>
@@ -5015,7 +5152,7 @@
       <c r="J51" s="4"/>
       <c r="K51" s="4"/>
     </row>
-    <row r="52" spans="1:11">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" s="18" t="s">
         <v>19</v>
       </c>
@@ -5043,7 +5180,7 @@
       <c r="J52" s="4"/>
       <c r="K52" s="4"/>
     </row>
-    <row r="53" spans="1:11">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" s="18" t="s">
         <v>19</v>
       </c>
@@ -5071,7 +5208,7 @@
       <c r="J53" s="4"/>
       <c r="K53" s="4"/>
     </row>
-    <row r="54" spans="1:11">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" s="18" t="s">
         <v>19</v>
       </c>
@@ -5098,7 +5235,7 @@
       <c r="J54" s="4"/>
       <c r="K54" s="4"/>
     </row>
-    <row r="55" spans="1:11">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" s="18" t="s">
         <v>19</v>
       </c>
@@ -5124,7 +5261,7 @@
       <c r="H55" s="4"/>
       <c r="K55" s="4"/>
     </row>
-    <row r="56" spans="1:11">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56" s="18" t="s">
         <v>19</v>
       </c>
@@ -5151,7 +5288,7 @@
       <c r="J56" s="4"/>
       <c r="K56" s="4"/>
     </row>
-    <row r="57" spans="1:11">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57" s="18" t="s">
         <v>19</v>
       </c>
@@ -5179,7 +5316,7 @@
       <c r="J57" s="4"/>
       <c r="K57" s="4"/>
     </row>
-    <row r="58" spans="1:11" s="10" customFormat="1">
+    <row r="58" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58" s="18" t="s">
         <v>76</v>
       </c>
@@ -5207,7 +5344,7 @@
       <c r="J58" s="4"/>
       <c r="K58" s="4"/>
     </row>
-    <row r="59" spans="1:11" s="10" customFormat="1">
+    <row r="59" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A59" s="18" t="s">
         <v>76</v>
       </c>
@@ -5235,7 +5372,7 @@
       <c r="J59" s="4"/>
       <c r="K59" s="4"/>
     </row>
-    <row r="60" spans="1:11" s="10" customFormat="1">
+    <row r="60" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60" s="18" t="s">
         <v>76</v>
       </c>
@@ -5263,7 +5400,7 @@
       <c r="J60" s="4"/>
       <c r="K60" s="4"/>
     </row>
-    <row r="61" spans="1:11" s="10" customFormat="1">
+    <row r="61" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61" s="18" t="s">
         <v>76</v>
       </c>
@@ -5291,7 +5428,7 @@
       <c r="J61" s="4"/>
       <c r="K61" s="4"/>
     </row>
-    <row r="62" spans="1:11">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62" s="18" t="s">
         <v>76</v>
       </c>
@@ -5315,7 +5452,7 @@
         <v>904</v>
       </c>
     </row>
-    <row r="63" spans="1:11">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63" s="18" t="s">
         <v>76</v>
       </c>
@@ -5339,7 +5476,7 @@
         <v>940</v>
       </c>
     </row>
-    <row r="64" spans="1:11">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64" s="18" t="s">
         <v>76</v>
       </c>
@@ -5363,7 +5500,7 @@
         <v>920</v>
       </c>
     </row>
-    <row r="65" spans="1:7">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" s="18" t="s">
         <v>76</v>
       </c>
@@ -5387,7 +5524,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="66" spans="1:7" s="10" customFormat="1">
+    <row r="66" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A66" s="18" t="s">
         <v>76</v>
       </c>
@@ -5411,7 +5548,7 @@
         <v>908</v>
       </c>
     </row>
-    <row r="67" spans="1:7" s="10" customFormat="1">
+    <row r="67" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A67" s="18" t="s">
         <v>76</v>
       </c>
@@ -5435,7 +5572,7 @@
         <v>891</v>
       </c>
     </row>
-    <row r="68" spans="1:7" s="10" customFormat="1">
+    <row r="68" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A68" s="18" t="s">
         <v>76</v>
       </c>
@@ -5459,7 +5596,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="69" spans="1:7" s="10" customFormat="1">
+    <row r="69" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A69" s="18" t="s">
         <v>76</v>
       </c>
@@ -5483,7 +5620,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="70" spans="1:7" s="10" customFormat="1">
+    <row r="70" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A70" s="18" t="s">
         <v>76</v>
       </c>
@@ -5507,7 +5644,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="71" spans="1:7" s="10" customFormat="1">
+    <row r="71" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A71" s="18" t="s">
         <v>76</v>
       </c>
@@ -5531,7 +5668,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="72" spans="1:7" s="10" customFormat="1">
+    <row r="72" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A72" s="18" t="s">
         <v>76</v>
       </c>
@@ -5555,7 +5692,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="73" spans="1:7">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" s="18" t="s">
         <v>76</v>
       </c>
@@ -5579,7 +5716,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="74" spans="1:7">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" s="18" t="s">
         <v>76</v>
       </c>
@@ -5603,7 +5740,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="75" spans="1:7">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" s="18" t="s">
         <v>76</v>
       </c>
@@ -5627,7 +5764,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="76" spans="1:7">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" s="18" t="s">
         <v>76</v>
       </c>
@@ -5651,7 +5788,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="77" spans="1:7" s="10" customFormat="1">
+    <row r="77" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A77" s="18" t="s">
         <v>76</v>
       </c>
@@ -5675,7 +5812,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="78" spans="1:7" s="10" customFormat="1">
+    <row r="78" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A78" s="18" t="s">
         <v>76</v>
       </c>
@@ -5699,7 +5836,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="79" spans="1:7" s="10" customFormat="1">
+    <row r="79" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A79" s="18" t="s">
         <v>76</v>
       </c>
@@ -5723,7 +5860,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="80" spans="1:7" s="10" customFormat="1">
+    <row r="80" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A80" s="18" t="s">
         <v>76</v>
       </c>
@@ -5747,7 +5884,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="81" spans="1:7" s="10" customFormat="1">
+    <row r="81" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A81" s="18" t="s">
         <v>76</v>
       </c>
@@ -5771,7 +5908,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="82" spans="1:7">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" s="18" t="s">
         <v>76</v>
       </c>
@@ -5795,7 +5932,7 @@
         <v>1180</v>
       </c>
     </row>
-    <row r="83" spans="1:7">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" s="18" t="s">
         <v>76</v>
       </c>
@@ -5819,7 +5956,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="84" spans="1:7">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" s="18" t="s">
         <v>76</v>
       </c>
@@ -5843,7 +5980,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="85" spans="1:7">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" s="18" t="s">
         <v>76</v>
       </c>
@@ -5867,7 +6004,7 @@
         <v>1210</v>
       </c>
     </row>
-    <row r="86" spans="1:7">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" s="18" t="s">
         <v>76</v>
       </c>
@@ -5891,7 +6028,7 @@
         <v>850</v>
       </c>
     </row>
-    <row r="87" spans="1:7">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" s="18" t="s">
         <v>76</v>
       </c>
@@ -5915,7 +6052,7 @@
         <v>870</v>
       </c>
     </row>
-    <row r="88" spans="1:7">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" s="18" t="s">
         <v>76</v>
       </c>
@@ -5939,7 +6076,7 @@
         <v>840</v>
       </c>
     </row>
-    <row r="89" spans="1:7">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" s="18" t="s">
         <v>76</v>
       </c>
@@ -5976,24 +6113,24 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L28"/>
+  <dimension ref="A1:L34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="G35" sqref="G35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.1640625" customWidth="1"/>
-    <col min="2" max="2" width="54.5" customWidth="1"/>
-    <col min="3" max="3" width="13.33203125" customWidth="1"/>
+    <col min="1" max="1" width="15.140625" customWidth="1"/>
+    <col min="2" max="2" width="54.42578125" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" customWidth="1"/>
     <col min="4" max="4" width="12" customWidth="1"/>
-    <col min="5" max="5" width="10.83203125" customWidth="1"/>
-    <col min="6" max="6" width="19.5" customWidth="1"/>
-    <col min="7" max="7" width="15.83203125" customWidth="1"/>
+    <col min="5" max="5" width="10.85546875" customWidth="1"/>
+    <col min="6" max="6" width="19.42578125" customWidth="1"/>
+    <col min="7" max="7" width="15.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>4</v>
       </c>
@@ -6021,7 +6158,7 @@
       <c r="K1" s="2"/>
       <c r="L1" s="2"/>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>40</v>
       </c>
@@ -6045,7 +6182,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>40</v>
       </c>
@@ -6062,14 +6199,14 @@
         <v>28</v>
       </c>
       <c r="F3" s="10">
-        <f t="shared" ref="F3:F20" si="0">(E3-D3)*70</f>
+        <f t="shared" ref="F3:F34" si="0">(E3-D3)*70</f>
         <v>70</v>
       </c>
       <c r="G3" s="10">
         <v>462</v>
       </c>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>40</v>
       </c>
@@ -6093,7 +6230,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="5" spans="1:12">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>40</v>
       </c>
@@ -6117,7 +6254,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="6" spans="1:12">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>40</v>
       </c>
@@ -6141,7 +6278,7 @@
         <v>878</v>
       </c>
     </row>
-    <row r="7" spans="1:12">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>40</v>
       </c>
@@ -6165,7 +6302,7 @@
         <v>878</v>
       </c>
     </row>
-    <row r="8" spans="1:12">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>40</v>
       </c>
@@ -6189,7 +6326,7 @@
         <v>878</v>
       </c>
     </row>
-    <row r="9" spans="1:12">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>40</v>
       </c>
@@ -6213,357 +6350,604 @@
         <v>878</v>
       </c>
     </row>
-    <row r="10" spans="1:12">
-      <c r="A10" t="s">
+    <row r="10" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="10" t="s">
         <v>71</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>144</v>
+        <v>225</v>
       </c>
       <c r="C10" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="D10">
-        <v>22</v>
-      </c>
-      <c r="E10">
+      <c r="D10" s="10">
+        <v>19</v>
+      </c>
+      <c r="E10" s="10">
         <v>29</v>
       </c>
       <c r="F10" s="10">
         <f t="shared" si="0"/>
-        <v>490</v>
-      </c>
-      <c r="G10">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12">
-      <c r="A11" t="s">
+        <v>700</v>
+      </c>
+      <c r="G10" s="10">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="10" t="s">
         <v>71</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>145</v>
+        <v>226</v>
       </c>
       <c r="C11" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="D11">
-        <v>23</v>
+      <c r="D11" s="10">
+        <v>20</v>
       </c>
       <c r="E11" s="10">
         <v>29</v>
       </c>
       <c r="F11" s="10">
         <f t="shared" si="0"/>
-        <v>420</v>
-      </c>
-      <c r="G11">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12">
+        <v>630</v>
+      </c>
+      <c r="G11" s="10">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>71</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C12" s="10" t="s">
         <v>9</v>
       </c>
       <c r="D12">
-        <v>24</v>
-      </c>
-      <c r="E12" s="10">
+        <v>22</v>
+      </c>
+      <c r="E12">
         <v>29</v>
       </c>
       <c r="F12" s="10">
         <f t="shared" si="0"/>
-        <v>350</v>
+        <v>490</v>
       </c>
       <c r="G12">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>71</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C13" s="10" t="s">
         <v>9</v>
       </c>
       <c r="D13">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E13" s="10">
         <v>29</v>
       </c>
       <c r="F13" s="10">
         <f t="shared" si="0"/>
-        <v>280</v>
+        <v>420</v>
       </c>
       <c r="G13">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>71</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C14" s="10" t="s">
         <v>9</v>
       </c>
       <c r="D14">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E14" s="10">
         <v>29</v>
       </c>
       <c r="F14" s="10">
         <f t="shared" si="0"/>
-        <v>210</v>
+        <v>350</v>
       </c>
       <c r="G14">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>71</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C15" s="10" t="s">
         <v>9</v>
       </c>
       <c r="D15">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E15" s="10">
         <v>29</v>
       </c>
       <c r="F15" s="10">
         <f t="shared" si="0"/>
-        <v>140</v>
+        <v>280</v>
       </c>
       <c r="G15">
-        <v>386</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12">
-      <c r="A16" s="10" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>71</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C16" s="10" t="s">
         <v>9</v>
       </c>
       <c r="D16">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E16" s="10">
         <v>29</v>
       </c>
       <c r="F16" s="10">
         <f t="shared" si="0"/>
-        <v>70</v>
+        <v>210</v>
       </c>
       <c r="G16">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7">
-      <c r="A17" s="10" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>71</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="D17" s="10">
-        <v>22</v>
+        <v>9</v>
+      </c>
+      <c r="D17">
+        <v>27</v>
       </c>
       <c r="E17" s="10">
         <v>29</v>
       </c>
       <c r="F17" s="10">
         <f t="shared" si="0"/>
-        <v>490</v>
+        <v>140</v>
       </c>
       <c r="G17">
-        <v>816</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="10" t="s">
         <v>71</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="D18" s="10">
-        <v>23</v>
+        <v>9</v>
+      </c>
+      <c r="D18">
+        <v>28</v>
       </c>
       <c r="E18" s="10">
         <v>29</v>
       </c>
       <c r="F18" s="10">
         <f t="shared" si="0"/>
-        <v>420</v>
+        <v>70</v>
       </c>
       <c r="G18">
-        <v>819</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="10" t="s">
         <v>71</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C19" s="10" t="s">
         <v>2</v>
       </c>
       <c r="D19" s="10">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E19" s="10">
         <v>29</v>
       </c>
       <c r="F19" s="10">
         <f t="shared" si="0"/>
-        <v>350</v>
+        <v>490</v>
       </c>
       <c r="G19">
-        <v>811</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7">
+        <v>816</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="10" t="s">
         <v>71</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C20" s="10" t="s">
         <v>2</v>
       </c>
       <c r="D20" s="10">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E20" s="10">
         <v>29</v>
       </c>
       <c r="F20" s="10">
         <f t="shared" si="0"/>
-        <v>280</v>
+        <v>420</v>
       </c>
       <c r="G20">
-        <v>760</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7">
+        <v>819</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="10" t="s">
         <v>71</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>155</v>
-      </c>
-      <c r="C21" t="s">
-        <v>10</v>
-      </c>
-      <c r="D21" s="10"/>
-    </row>
-    <row r="22" spans="1:7">
+        <v>153</v>
+      </c>
+      <c r="C21" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D21" s="10">
+        <v>24</v>
+      </c>
+      <c r="E21" s="10">
+        <v>29</v>
+      </c>
+      <c r="F21" s="10">
+        <f t="shared" si="0"/>
+        <v>350</v>
+      </c>
+      <c r="G21">
+        <v>811</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
         <v>71</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7">
+        <v>2</v>
+      </c>
+      <c r="D22" s="10">
+        <v>25</v>
+      </c>
+      <c r="E22" s="10">
+        <v>29</v>
+      </c>
+      <c r="F22" s="10">
+        <f t="shared" si="0"/>
+        <v>280</v>
+      </c>
+      <c r="G22">
+        <v>760</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="10" t="s">
         <v>71</v>
       </c>
       <c r="B23" s="10" t="s">
-        <v>157</v>
-      </c>
-      <c r="C23" s="10" t="s">
+        <v>155</v>
+      </c>
+      <c r="C23" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="24" spans="1:7">
+      <c r="D23" s="10">
+        <v>21</v>
+      </c>
+      <c r="E23" s="10">
+        <v>29</v>
+      </c>
+      <c r="F23">
+        <f t="shared" si="0"/>
+        <v>560</v>
+      </c>
+      <c r="G23">
+        <v>1100</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="10" t="s">
         <v>71</v>
       </c>
       <c r="B24" s="10" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C24" s="10" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="25" spans="1:7">
+      <c r="D24" s="10">
+        <v>22</v>
+      </c>
+      <c r="E24" s="10">
+        <v>29</v>
+      </c>
+      <c r="F24" s="10">
+        <f t="shared" si="0"/>
+        <v>490</v>
+      </c>
+      <c r="G24">
+        <v>1100</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="10" t="s">
         <v>71</v>
       </c>
       <c r="B25" s="10" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C25" s="10" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="26" spans="1:7">
+      <c r="D25" s="10">
+        <v>23</v>
+      </c>
+      <c r="E25" s="10">
+        <v>29</v>
+      </c>
+      <c r="F25" s="10">
+        <f t="shared" si="0"/>
+        <v>420</v>
+      </c>
+      <c r="G25">
+        <v>1095</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="10" t="s">
         <v>71</v>
       </c>
       <c r="B26" s="10" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C26" s="10" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="27" spans="1:7">
+      <c r="D26" s="10">
+        <v>24</v>
+      </c>
+      <c r="E26" s="10">
+        <v>29</v>
+      </c>
+      <c r="F26" s="10">
+        <f t="shared" si="0"/>
+        <v>350</v>
+      </c>
+      <c r="G26">
+        <v>1095</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="10" t="s">
         <v>71</v>
       </c>
       <c r="B27" s="10" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C27" s="10" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="28" spans="1:7">
+      <c r="D27">
+        <v>25</v>
+      </c>
+      <c r="E27" s="10">
+        <v>29</v>
+      </c>
+      <c r="F27" s="10">
+        <f t="shared" si="0"/>
+        <v>280</v>
+      </c>
+      <c r="G27">
+        <v>1076</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="10" t="s">
         <v>71</v>
       </c>
       <c r="B28" s="10" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C28" s="10" t="s">
         <v>10</v>
+      </c>
+      <c r="D28">
+        <v>26</v>
+      </c>
+      <c r="E28" s="10">
+        <v>29</v>
+      </c>
+      <c r="F28" s="10">
+        <f t="shared" si="0"/>
+        <v>210</v>
+      </c>
+      <c r="G28">
+        <v>1065</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="B29" s="10" t="s">
+        <v>161</v>
+      </c>
+      <c r="C29" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D29">
+        <v>27</v>
+      </c>
+      <c r="E29" s="10">
+        <v>29</v>
+      </c>
+      <c r="F29" s="10">
+        <f t="shared" si="0"/>
+        <v>140</v>
+      </c>
+      <c r="G29">
+        <v>1055</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="B30" s="10" t="s">
+        <v>162</v>
+      </c>
+      <c r="C30" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D30">
+        <v>28</v>
+      </c>
+      <c r="E30" s="10">
+        <v>29</v>
+      </c>
+      <c r="F30" s="10">
+        <f t="shared" si="0"/>
+        <v>70</v>
+      </c>
+      <c r="G30">
+        <v>1065</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="B31" s="10" t="s">
+        <v>227</v>
+      </c>
+      <c r="C31" t="s">
+        <v>46</v>
+      </c>
+      <c r="D31">
+        <v>30</v>
+      </c>
+      <c r="E31" s="10">
+        <v>29</v>
+      </c>
+      <c r="F31" s="10">
+        <f t="shared" si="0"/>
+        <v>-70</v>
+      </c>
+      <c r="G31">
+        <v>681</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="B32" s="10" t="s">
+        <v>228</v>
+      </c>
+      <c r="C32" t="s">
+        <v>46</v>
+      </c>
+      <c r="D32">
+        <v>31</v>
+      </c>
+      <c r="E32" s="10">
+        <v>29</v>
+      </c>
+      <c r="F32" s="10">
+        <f t="shared" si="0"/>
+        <v>-140</v>
+      </c>
+      <c r="G32">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="B33" s="10" t="s">
+        <v>229</v>
+      </c>
+      <c r="C33" t="s">
+        <v>46</v>
+      </c>
+      <c r="D33">
+        <v>32</v>
+      </c>
+      <c r="E33" s="10">
+        <v>29</v>
+      </c>
+      <c r="F33" s="10">
+        <f t="shared" si="0"/>
+        <v>-210</v>
+      </c>
+      <c r="G33">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="B34" s="10" t="s">
+        <v>230</v>
+      </c>
+      <c r="C34" t="s">
+        <v>46</v>
+      </c>
+      <c r="D34">
+        <v>33</v>
+      </c>
+      <c r="E34" s="10">
+        <v>29</v>
+      </c>
+      <c r="F34" s="10">
+        <f t="shared" si="0"/>
+        <v>-280</v>
+      </c>
+      <c r="G34">
+        <v>637</v>
       </c>
     </row>
   </sheetData>
@@ -6579,31 +6963,32 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L17"/>
+  <dimension ref="A1:AQ19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="I1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="L17" sqref="L17"/>
+    <sheetView topLeftCell="A12" zoomScale="99" zoomScaleNormal="99" zoomScalePageLayoutView="120" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="P18" sqref="P18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="62" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="62.1" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.5" style="6" customWidth="1"/>
+    <col min="1" max="1" width="15.42578125" style="6" customWidth="1"/>
     <col min="2" max="2" width="17" style="6" customWidth="1"/>
-    <col min="3" max="3" width="9.1640625" style="6" customWidth="1"/>
-    <col min="4" max="4" width="10.5" style="6" customWidth="1"/>
-    <col min="5" max="5" width="14.6640625" style="6" customWidth="1"/>
-    <col min="6" max="6" width="29.6640625" style="6" customWidth="1"/>
-    <col min="7" max="7" width="15.5" style="6" customWidth="1"/>
-    <col min="8" max="8" width="14.1640625" style="6" customWidth="1"/>
-    <col min="9" max="9" width="13.1640625" style="6" customWidth="1"/>
-    <col min="10" max="10" width="12.6640625" style="6" customWidth="1"/>
-    <col min="11" max="11" width="52.1640625" style="6" customWidth="1"/>
-    <col min="12" max="12" width="44.6640625" style="6" customWidth="1"/>
-    <col min="13" max="16384" width="8.83203125" style="6"/>
+    <col min="3" max="3" width="9.140625" style="6" customWidth="1"/>
+    <col min="4" max="4" width="10.42578125" style="6" customWidth="1"/>
+    <col min="5" max="5" width="14.7109375" style="6" customWidth="1"/>
+    <col min="6" max="6" width="29.7109375" style="6" customWidth="1"/>
+    <col min="7" max="7" width="15.42578125" style="6" customWidth="1"/>
+    <col min="8" max="8" width="14.140625" style="6" customWidth="1"/>
+    <col min="9" max="9" width="13.140625" style="6" customWidth="1"/>
+    <col min="10" max="10" width="12.7109375" style="6" customWidth="1"/>
+    <col min="11" max="11" width="52.140625" style="6" customWidth="1"/>
+    <col min="12" max="12" width="44.7109375" style="6" customWidth="1"/>
+    <col min="13" max="13" width="12.7109375" style="6" customWidth="1"/>
+    <col min="14" max="16384" width="8.85546875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="7" customFormat="1" ht="44" customHeight="1">
+    <row r="1" spans="1:43" s="7" customFormat="1" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>54</v>
       </c>
@@ -6641,7 +7026,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="2" spans="1:12" s="9" customFormat="1" ht="62" customHeight="1">
+    <row r="2" spans="1:43" s="9" customFormat="1" ht="62.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>1</v>
       </c>
@@ -6676,7 +7061,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="62" customHeight="1">
+    <row r="3" spans="1:43" ht="62.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
         <v>17</v>
       </c>
@@ -6714,7 +7099,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="62" customHeight="1">
+    <row r="4" spans="1:43" ht="62.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>18</v>
       </c>
@@ -6752,7 +7137,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="62" customHeight="1">
+    <row r="5" spans="1:43" ht="62.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
         <v>19</v>
       </c>
@@ -6787,7 +7172,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="62" customHeight="1">
+    <row r="6" spans="1:43" ht="62.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
         <v>76</v>
       </c>
@@ -6813,7 +7198,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="62" customHeight="1">
+    <row r="7" spans="1:43" ht="62.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
         <v>27</v>
       </c>
@@ -6848,7 +7233,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="62" customHeight="1">
+    <row r="8" spans="1:43" ht="62.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
         <v>31</v>
       </c>
@@ -6883,7 +7268,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="62" customHeight="1">
+    <row r="9" spans="1:43" ht="62.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
         <v>32</v>
       </c>
@@ -6921,7 +7306,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="62" customHeight="1">
+    <row r="10" spans="1:43" ht="62.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
         <v>33</v>
       </c>
@@ -6956,7 +7341,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="92" customHeight="1">
+    <row r="11" spans="1:43" ht="92.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
         <v>34</v>
       </c>
@@ -6994,7 +7379,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="75" customHeight="1">
+    <row r="12" spans="1:43" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
         <v>35</v>
       </c>
@@ -7029,7 +7414,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="62" customHeight="1">
+    <row r="13" spans="1:43" ht="62.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>40</v>
       </c>
@@ -7061,87 +7446,324 @@
         <v>184</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="62" customHeight="1">
-      <c r="A14" s="6" t="s">
+    <row r="14" spans="1:43" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="23" t="s">
         <v>71</v>
       </c>
-      <c r="B14" s="6" t="s">
+      <c r="B14" s="23" t="s">
         <v>65</v>
       </c>
-      <c r="C14" s="6" t="s">
+      <c r="C14" s="23" t="s">
         <v>69</v>
       </c>
-      <c r="D14" s="14">
+      <c r="D14" s="24">
         <v>42108</v>
       </c>
-      <c r="E14" s="14">
+      <c r="E14" s="24">
         <v>42167</v>
       </c>
-      <c r="F14" s="6" t="s">
+      <c r="F14" s="23" t="s">
         <v>64</v>
       </c>
-      <c r="K14" s="6" t="s">
+      <c r="G14" s="23"/>
+      <c r="H14" s="23"/>
+      <c r="I14" s="23"/>
+      <c r="J14" s="23"/>
+      <c r="K14" s="23" t="s">
         <v>188</v>
       </c>
-      <c r="L14" s="6" t="s">
+      <c r="L14" s="23" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="15" spans="1:12" ht="62" customHeight="1">
-      <c r="A15" s="6" t="s">
+      <c r="M14" s="22" t="s">
+        <v>77</v>
+      </c>
+      <c r="N14" s="22" t="s">
+        <v>190</v>
+      </c>
+      <c r="O14" s="22" t="s">
+        <v>191</v>
+      </c>
+      <c r="P14" s="22" t="s">
+        <v>192</v>
+      </c>
+      <c r="Q14" s="22" t="s">
+        <v>193</v>
+      </c>
+      <c r="R14" s="22" t="s">
+        <v>194</v>
+      </c>
+      <c r="S14" s="22" t="s">
+        <v>195</v>
+      </c>
+      <c r="T14" s="22" t="s">
+        <v>196</v>
+      </c>
+      <c r="U14" s="22" t="s">
+        <v>197</v>
+      </c>
+      <c r="V14" s="22" t="s">
+        <v>198</v>
+      </c>
+      <c r="W14" s="22" t="s">
+        <v>199</v>
+      </c>
+      <c r="X14" s="22" t="s">
+        <v>200</v>
+      </c>
+      <c r="Y14" s="22" t="s">
+        <v>201</v>
+      </c>
+      <c r="Z14" s="22" t="s">
+        <v>202</v>
+      </c>
+      <c r="AA14" s="22" t="s">
+        <v>203</v>
+      </c>
+      <c r="AB14" s="22" t="s">
+        <v>204</v>
+      </c>
+      <c r="AC14" s="22" t="s">
+        <v>205</v>
+      </c>
+      <c r="AD14" s="22" t="s">
+        <v>206</v>
+      </c>
+      <c r="AE14" s="22" t="s">
+        <v>207</v>
+      </c>
+      <c r="AF14" s="22" t="s">
+        <v>208</v>
+      </c>
+      <c r="AG14" s="22" t="s">
+        <v>209</v>
+      </c>
+      <c r="AH14" s="22" t="s">
+        <v>210</v>
+      </c>
+      <c r="AI14" s="22" t="s">
+        <v>211</v>
+      </c>
+      <c r="AJ14" s="22" t="s">
+        <v>212</v>
+      </c>
+      <c r="AK14" s="22" t="s">
+        <v>213</v>
+      </c>
+      <c r="AL14" s="22" t="s">
+        <v>214</v>
+      </c>
+      <c r="AM14" s="22" t="s">
+        <v>215</v>
+      </c>
+      <c r="AN14" s="22" t="s">
+        <v>216</v>
+      </c>
+      <c r="AO14" s="22" t="s">
+        <v>217</v>
+      </c>
+      <c r="AP14" s="22" t="s">
+        <v>218</v>
+      </c>
+      <c r="AQ14" s="22" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="15" spans="1:43" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="23"/>
+      <c r="B15" s="23"/>
+      <c r="C15" s="23"/>
+      <c r="D15" s="24"/>
+      <c r="E15" s="24"/>
+      <c r="F15" s="23"/>
+      <c r="G15" s="23"/>
+      <c r="H15" s="23"/>
+      <c r="I15" s="23"/>
+      <c r="J15" s="23"/>
+      <c r="K15" s="23"/>
+      <c r="L15" s="23"/>
+      <c r="M15" s="22" t="s">
+        <v>220</v>
+      </c>
+      <c r="N15" s="22">
+        <v>0</v>
+      </c>
+      <c r="O15" s="22">
+        <v>0</v>
+      </c>
+      <c r="P15" s="22">
+        <v>0</v>
+      </c>
+      <c r="Q15" s="22">
+        <v>0</v>
+      </c>
+      <c r="R15" s="22">
+        <v>0</v>
+      </c>
+      <c r="S15" s="22">
+        <v>0</v>
+      </c>
+      <c r="T15" s="22">
+        <v>-1</v>
+      </c>
+      <c r="U15" s="22">
+        <v>-1</v>
+      </c>
+      <c r="V15" s="22">
+        <v>-1</v>
+      </c>
+      <c r="W15" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="X15" s="22" t="s">
+        <v>222</v>
+      </c>
+      <c r="Y15" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="Z15" s="22" t="s">
+        <v>222</v>
+      </c>
+      <c r="AA15" s="22" t="s">
+        <v>222</v>
+      </c>
+      <c r="AB15" s="22" t="s">
+        <v>222</v>
+      </c>
+      <c r="AC15" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="AD15" s="22" t="s">
+        <v>223</v>
+      </c>
+      <c r="AE15" s="22" t="s">
+        <v>222</v>
+      </c>
+      <c r="AF15" s="22" t="s">
+        <v>222</v>
+      </c>
+      <c r="AG15" s="22" t="s">
+        <v>222</v>
+      </c>
+      <c r="AH15" s="22" t="s">
+        <v>222</v>
+      </c>
+      <c r="AI15" s="22" t="s">
+        <v>222</v>
+      </c>
+      <c r="AJ15" s="22" t="s">
+        <v>223</v>
+      </c>
+      <c r="AK15" s="22" t="s">
+        <v>222</v>
+      </c>
+      <c r="AL15" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="AM15" s="22" t="s">
+        <v>223</v>
+      </c>
+      <c r="AN15" s="22" t="s">
+        <v>222</v>
+      </c>
+      <c r="AO15" s="22" t="s">
+        <v>222</v>
+      </c>
+      <c r="AP15" s="22" t="s">
+        <v>222</v>
+      </c>
+      <c r="AQ15" s="22" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="16" spans="1:43" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="23"/>
+      <c r="B16" s="23"/>
+      <c r="C16" s="23"/>
+      <c r="D16" s="24"/>
+      <c r="E16" s="24"/>
+      <c r="F16" s="23"/>
+      <c r="G16" s="23"/>
+      <c r="H16" s="23"/>
+      <c r="I16" s="23"/>
+      <c r="J16" s="23"/>
+      <c r="K16" s="23"/>
+      <c r="L16" s="23"/>
+      <c r="M16" s="22" t="s">
+        <v>224</v>
+      </c>
+      <c r="N16" s="22"/>
+      <c r="O16" s="22"/>
+      <c r="P16" s="22"/>
+      <c r="Q16" s="22"/>
+      <c r="R16" s="22"/>
+      <c r="S16" s="22"/>
+      <c r="T16" s="22"/>
+      <c r="U16" s="22"/>
+      <c r="V16" s="22"/>
+      <c r="W16" s="22"/>
+      <c r="X16" s="22"/>
+      <c r="Y16" s="22" t="s">
+        <v>223</v>
+      </c>
+      <c r="Z16" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="AA16" s="22" t="s">
+        <v>223</v>
+      </c>
+      <c r="AB16" s="22" t="s">
+        <v>223</v>
+      </c>
+      <c r="AC16" s="22" t="s">
+        <v>223</v>
+      </c>
+      <c r="AD16" s="22" t="s">
+        <v>223</v>
+      </c>
+      <c r="AE16" s="22" t="s">
+        <v>223</v>
+      </c>
+      <c r="AF16" s="22" t="s">
+        <v>222</v>
+      </c>
+      <c r="AG16" s="22" t="s">
+        <v>222</v>
+      </c>
+      <c r="AH16" s="22" t="s">
+        <v>222</v>
+      </c>
+      <c r="AI16" s="22" t="s">
+        <v>222</v>
+      </c>
+      <c r="AJ16" s="22" t="s">
+        <v>222</v>
+      </c>
+      <c r="AK16" s="22" t="s">
+        <v>222</v>
+      </c>
+      <c r="AL16" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="AM16" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="AN16" s="22" t="s">
+        <v>222</v>
+      </c>
+      <c r="AO16" s="22" t="s">
+        <v>223</v>
+      </c>
+      <c r="AP16" s="22" t="s">
+        <v>223</v>
+      </c>
+      <c r="AQ16" s="22" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="81" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="6" t="s">
         <v>72</v>
-      </c>
-      <c r="B15" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="D15" s="14">
-        <v>42108</v>
-      </c>
-      <c r="E15" s="14">
-        <v>42167</v>
-      </c>
-      <c r="F15" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="K15" s="6" t="s">
-        <v>188</v>
-      </c>
-      <c r="L15" s="6" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" ht="62" customHeight="1">
-      <c r="A16" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="B16" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="C16" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="D16" s="14">
-        <v>42108</v>
-      </c>
-      <c r="E16" s="14">
-        <v>42167</v>
-      </c>
-      <c r="F16" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="K16" s="6" t="s">
-        <v>186</v>
-      </c>
-      <c r="L16" s="6" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" ht="62" customHeight="1">
-      <c r="A17" s="6" t="s">
-        <v>74</v>
       </c>
       <c r="B17" s="6" t="s">
         <v>65</v>
@@ -7156,16 +7778,82 @@
         <v>42167</v>
       </c>
       <c r="F17" s="6" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="K17" s="6" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="L17" s="6" t="s">
         <v>184</v>
       </c>
     </row>
+    <row r="18" spans="1:12" ht="62.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="D18" s="14">
+        <v>42108</v>
+      </c>
+      <c r="E18" s="14">
+        <v>42167</v>
+      </c>
+      <c r="F18" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="K18" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="L18" s="6" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="62.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="D19" s="14">
+        <v>42108</v>
+      </c>
+      <c r="E19" s="14">
+        <v>42167</v>
+      </c>
+      <c r="F19" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="K19" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="L19" s="6" t="s">
+        <v>184</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="12">
+    <mergeCell ref="L14:L16"/>
+    <mergeCell ref="A14:A16"/>
+    <mergeCell ref="B14:B16"/>
+    <mergeCell ref="C14:C16"/>
+    <mergeCell ref="D14:D16"/>
+    <mergeCell ref="E14:E16"/>
+    <mergeCell ref="F14:F16"/>
+    <mergeCell ref="G14:G16"/>
+    <mergeCell ref="H14:H16"/>
+    <mergeCell ref="I14:I16"/>
+    <mergeCell ref="J14:J16"/>
+    <mergeCell ref="K14:K16"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295"/>
   <extLst>

</xml_diff>